<commit_message>
added exception if value is null
add 'null' then remove it before export
</commit_message>
<xml_diff>
--- a/ingredients/ingredients.xlsx
+++ b/ingredients/ingredients.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\englishTranslate\ingredients\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A0D983-A77F-439D-9066-43119FE9F005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC4F90E-5404-466A-B5BD-9178911489C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{277A9B31-7E86-49C3-9996-15C89BA3B75E}"/>
   </bookViews>
@@ -16,26 +16,19 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$82</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$164</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="129">
   <si>
     <t>ingredients_ori</t>
   </si>
@@ -46,21 +39,9 @@
     <t>小麦粉(国内製造)、植物油脂、しょうゆ、砂糖、食塩、チキンエキス、たんぱく加水分解物、ミート調味エキス、ミート調味パウダー、酵母エキスパウダー、ポークパウダー、魚介パウダー/加工デンプン、調味料(アミノ酸等）、炭酸Ca、酸化防止剤（ビタミンE）、（一部に小麦・大豆・鶏肉・豚肉・ゼラチンを含む）</t>
   </si>
   <si>
-    <t>乾燥ポテト（外国製造）、植物油脂、食塩（美ら海育ち15%）／加工澱粉、調味料（アミノ酸等）、香料、酸化防止剤（ビタミンE）</t>
-  </si>
-  <si>
     <t>砂糖（国内製造又は外国製造）、小麦粉、植物油脂、カカオマス、でん粉、ショートニング、乳糖、全粉乳、液卵、ホエイパウダー、クリームパウダー、脱脂粉乳、食塩、ココアパウダー、ココアバター／炭酸Ｃａ、膨脹剤、カラメル色素、乳化剤（大豆由来）、香料</t>
   </si>
   <si>
-    <t>乾燥ポテト（外国製造）、植物油脂、唐辛子パウダー、食塩、ガーリックパウダー、オニオンパウダー、砂糖、酵母エキスパウダー、ガーリック風味パウダー、たんぱく加水分解物、ブドウ糖、野菜エキスパウダー、チリパウダー、チキンパウダー、乳糖、ホワイトペッパーパウダー、クミンパウダー、パプリカパウダー、ハバネロペースト／加工澱粉、調味料（アミノ酸等）、炭酸Ca、香料、カロチノイド色素、酸化防止剤（ビタミンE）、香辛料抽出物、酸味料、カラメル色素、（一部に乳成分・小麦・ごま・大豆・鶏肉・豚肉を含む）</t>
-  </si>
-  <si>
-    <t>小麦粉（国内製造）、砂糖、アーモンド、全粉乳、植物油脂、カカオマス、ココアバター、小麦全粒粉、ショートニング、アーモンドプラリネペースト、小麦たんぱく、食塩、イースト／乳化剤、香料、膨脹剤、（一部に乳成分・小麦・大豆・アーモンドを含む）</t>
-  </si>
-  <si>
-    <t>小麦粉（国内製造）、植物油脂、アーモンド、でん粉、砂糖、オニオンペースト、ポークエキスパウダー、ショートニング、にんにくパウダー、モルトエキス、チキンエキスパウダー、小麦たんぱく、食塩、しょうゆシーズニング、こしょう、乾燥ビール酵母、酵母エキスパウダー、ベーコンエキス、たまねぎシーズニング、イースト／加工デンプン、調味料（アミノ酸等）、香料、乳化剤、くん液、（一部に乳成分・小麦・大豆・鶏肉・豚肉・ごま・アーモンドを含む）</t>
-  </si>
-  <si>
     <t>砂糖（外国製造又は国内製造）、小麦粉、植物油脂、全粉乳、カカオマス、乳糖、ココアバター、ショートニング、ココアパウダー、加糖脱脂練乳、異性化液糖、生クリーム、食塩／乳化剤、膨脹剤、香料、着色料(カラメル)、（一部に乳成分・小麦・大豆を含む）</t>
   </si>
   <si>
@@ -79,30 +60,9 @@
     <t>油揚げめん（小麦粉（国内製造）、植物油脂、食塩、香辛料、粉末野菜、卵白）、添付調味料（チキンエキス、しょうゆ、食塩、植物油、発酵調味料、砂糖、野菜エキス、こんぶエキス、香辛料、酵母エキス、鶏脂、ラード、魚介エキス）、かやく（ワンタン、卵）／加工でん粉、調味料（アミノ酸等）、酒精、炭酸カルシウム、かんすい、酸化防止剤（ビタミンＣ、ビタミンＥ）、レシチン、クチナシ色素、カラメル色素、増粘多糖類、カロチン色素、ビタミンＢ２、ビタミンＢ１、（一部に小麦・卵・乳成分・ごま・大豆・鶏肉・豚肉・ゼラチンを含む）</t>
   </si>
   <si>
-    <t>砂糖（タイ製造）、水あめ、ゼラチン、食用油脂／甘味料（ソルビトール）、酸味料、香料、ゲル化剤（ペクチン：オレンジ由来）、着色料（クチナシ、野菜色素）</t>
-  </si>
-  <si>
-    <t>小麦粉（国内製造）、砂糖、ショートニング、抹茶（京都産宇治抹茶100%）、食塩、乳糖／膨張剤、クチナシ色素、香料、乳化剤（大豆由来）、酸化防止剤（ビタミンE）</t>
-  </si>
-  <si>
-    <t>小麦粉（国内製造）、砂糖、ココナッツオイル、ショートニング、玄米粉、食塩、ココナッツ、梅干しエキスパウダー、コーンスターチ、乳糖/膨張剤、酸味料、乳化剤（大豆由来）、香料</t>
-  </si>
-  <si>
-    <t>小麦粉（国内製造）、砂糖、ココナッツオイル、ショートニング、玄米粉、醤油風味シーズニング（大豆を含む）、ココナッツ、食塩、乳糖/膨張剤、調味料（アミノ酸）、乳化剤、カラメル色素</t>
-  </si>
-  <si>
-    <t>砂糖（国内製造）、果糖ぶどう糖液糖、パラチノース、ぶどう糖、 添加物：酸味料、ゲル化剤（増粘多糖類）、乳酸Ca、香料、V.B2、V.B1、V.B6</t>
-  </si>
-  <si>
-    <t>チョコレート（砂糖、全粉乳、植物油脂、ココアバター、カカオマス、乳糖）、ウエハース（小麦粉、砂糖、でんぷん、植物油脂、食塩）/加工でんぷん、乳化剤（大豆由来）、貝カルシウム、香料、着色料（カラメル）、膨張剤</t>
-  </si>
-  <si>
     <t>チョコレート（乳糖、ココアバター、砂糖、植物油脂、全粉乳、乾燥いちご）、ウエハース（小麦粉、砂糖、でんぷん、植物油脂、食塩）/加工でんぷん、香料、乳化剤（大豆由来）、着色料（アカビート、紅麹）貝カルシウム、膨張剤、酸味料</t>
   </si>
   <si>
-    <t>砂糖（国内製造）／ゲル化剤（増粘多糖類）、香料、酸味料、リン酸Ca、着色料（クチナシ）</t>
-  </si>
-  <si>
     <t>水飴、砂糖、澱粉、餅粉、植物油、ソルビトール、乳化剤、香料、酸味料、着色料（赤１０６）</t>
   </si>
   <si>
@@ -112,51 +72,15 @@
     <t>果糖ぶどう糖液糖､香料､酸味料</t>
   </si>
   <si>
-    <t>果糖ぶどう糖液糖、酸味料、香料</t>
-  </si>
-  <si>
     <t>砂糖（国内製造）、小麦粉、植物油脂、乳糖、でん粉、ショートニング、ココアバター、全粉乳、ホエイパウダー、液卵、マルチトール、ストロベリーパウダー、クリームパウダー、食塩／炭酸Ｃａ、膨脹剤、着色料（カラメル、紅麹、アカビート）、香料、乳化剤（大豆由来）</t>
   </si>
   <si>
-    <t>砂糖（国内製造又は韓国製造）、小麦粉、植物油脂、全粉乳、乳糖、カカオマス、ホエイパウダー、クッキークランチ、ココアパウダー、でん粉、ショートニング、食塩／乳化剤（大豆由来）、カラメル色素、膨脹剤、香料</t>
-  </si>
-  <si>
-    <t>水飴（国内製造）、砂糖、植物油脂、ぶどう濃縮果汁／酸味料、香料、着色料（アントシアニン、クチナシ、紅麹、金箔）、チャ抽出物、タンニン（抽出物）、乳化剤</t>
-  </si>
-  <si>
     <t>油揚げめん（小麦粉（国内製造）、植物油脂、ラード、食塩、植物性たん白、しょうゆ）、スープ（しょうゆ、糖類、食塩、動物油脂、ビーフエキス、たん白加水分解物、昆布エキス、鰹エキス）、かやく（かす入り揚げ玉、とろろ昆布、かまぼこ、ねぎ）／加工でん粉、調味料（アミノ酸等）、酒精、リン酸Na、香料、増粘剤（キサンタン）、酸化防止剤（ビタミンE)、カラメル色素、膨脹剤、紅麹色素、クチナシ色素、（一部に小麦・牛肉・大豆・鶏肉・豚肉を含む）</t>
   </si>
   <si>
-    <t>馬鈴薯（国産）（遺伝子組換えでない）、植物油脂、ショートニング、乳糖、砂糖、食塩、チーズパウダー、デキストリン、クリーミングパウダー、ぶどう糖、オニオンパウダー、酒粕パウダー、酵母エキスパウダー、しょうゆパウダー／調味料（アミノ酸等）、香料、加工デンプン、乳化剤、着色料（カロチノイド、カラメル）、酸味料、甘味料（スクラロース）、香辛料抽出物、（一部に小麦・乳成分・大豆を含む）</t>
-  </si>
-  <si>
-    <t>油揚げめん（小麦粉（国内製造）、植物油脂、ラード、食塩、香辛料）、添付調味料（たん白加水分解物、しょうゆ、糖類、かつお節エキス、魚介エキス、食塩、いりこ、かつお節）、かやく（揚げ玉、ねぎ）/加工デンプン、調味料（アミノ酸等）、トレハロース、酒精、増粘多糖類、酸化防止剤（ビタミンE)、膨張剤、香辛料抽出物、（一部に小麦・さば・大豆を含む）</t>
-  </si>
-  <si>
-    <t>砂糖・ぶどう糖果糖液糖（国内製造）/炭酸ガス、香料、酸味料</t>
-  </si>
-  <si>
     <t>砂糖、ぶどう糖果糖液糖(国内製造)/炭酸ガス、酸味料、香料</t>
   </si>
   <si>
-    <t>砂糖混合ぶどう糖果糖液糖、酸味料、香料、着色料（赤色40号）</t>
-  </si>
-  <si>
-    <t>砂糖混合ぶどう糖果糖液糖、酸味料、香料、着色料（黄色4号、青色1号）</t>
-  </si>
-  <si>
-    <t>砂糖混合ぶどう糖果糖液糖、酸味料、香料、着色料（青色1号）</t>
-  </si>
-  <si>
-    <t>砂糖混合ぶどう糖果糖液糖、酸味料、香料、着色料（黄色4号、赤色40号）</t>
-  </si>
-  <si>
-    <t>砂糖・ぶどう糖果糖液糖（国内製造）/炭酸ガス、酸味料、香料</t>
-  </si>
-  <si>
-    <t>砂糖・ぶどう糖果糖液糖/炭酸ガス、酸味料、香料 、着色料（黄色4号、 青色1号）</t>
-  </si>
-  <si>
     <t>緑茶（国産）／ビタミンＣ</t>
   </si>
   <si>
@@ -166,9 +90,6 @@
     <t>砂糖、粉末麦芽調製品（混合麦芽エキス、砂糖、ココアパウダー、脱脂粉乳、植物油脂、乳清カルシウム）、モルトエキス、ココアパウダー、脱脂粉乳、乳化剤、炭酸カルシウム、炭酸マグネシウム、ビタミンC、ビタミンD、ｐH調整剤、ピロリン酸鉄、レシチン（大豆由来）、ナイアシン、ビタミンB1、酸化防止剤（ビタミンE）、ビタミンB2、ビタミンA</t>
   </si>
   <si>
-    <t>コーングリッツ（国内製造）、砂糖、植物油脂、マーガリン、牛乳、抹茶、加糖れん乳、食塩、抹茶ペースト／ソルビトール、香料、乳化剤、カロチノイド色素、（一部に乳成分・大豆を含む）</t>
-  </si>
-  <si>
     <t>砂糖、植物油脂、コーングリッツ（遺伝子組換えでない）、パン粉、マーガリン、ココアパウダー、加糖れん乳、カラメルソース、食塩、クリーム（乳製品）、発酵風味パウダー、乳糖、カカオマス、全粉乳、クリーム粉末、卵殻未焼成Ｃａ、カラメル色素、香料、乳化剤、トレハロース、（原材料の一部に大豆を含む）</t>
   </si>
   <si>
@@ -178,291 +99,33 @@
     <t>コーングリッツ（遺伝子組換えでない）、砂糖、植物油脂、マーガリン、ココアパウダー、加糖れん乳、カラメルソース、食塩、クリーム（乳製品）、発酵風味パウダー、乳糖、カカオマス、全粉乳、たんぱく加水分解物、クリーム粉末、カラメル色素、卵殻未焼成Ca、香料、乳化剤、トレハロース、（原材料の一部に小麦、大豆を含む）</t>
   </si>
   <si>
-    <t>乾燥ポテト（外国製造）、植物油脂、食塩、オニオンパウダー、チキンエキスパウダー、ブドウ糖、酵母エキスパウダー、ポークエキス調味料、粉末醤油、砂糖、ミルポアパウダー、香辛料、粉末ソース、粉末みそ、粉末野菜調味料、トマトパウダー、キャロットパウダー／加工澱粉、調味料（アミノ酸等）、甘味料（ステビア、スクラロース）、炭酸Ca、酸味料、酸化防止剤（ビタミンE）、香料、カラメル色素、香辛料抽出物、（一部に乳成分・小麦・大豆・鶏肉・豚肉・ゼラチンを含む）</t>
-  </si>
-  <si>
-    <t>乾燥ポテト（外国製造）、植物油脂、食塩（焼き塩62％）、粉末油脂、ブドウ糖、オニオンパウダー、焙煎玄米粉、ロースト醤油風味パウダー、ガーリックパウダー、酵母エキスパウダー／加工澱粉、調味料（アミノ酸等）、炭酸Ca、香料、酸化防止剤（ビタミンE）、（一部に乳成分・小麦・大豆を含む）</t>
-  </si>
-  <si>
-    <t>水あめ、砂糖、ゼラチン、濃縮果汁（バナナ、レモン、すもも）、植物油脂／ソルビトール、酸味料、骨Ca、香料、着色料（アントシアニン、クチナシ）、光沢剤、（一部にバナナ・ゼラチンを含む）</t>
-  </si>
-  <si>
-    <t>水あめ（国内製造）、砂糖、ゼラチン、植物油脂／ソルビトール、酸味料、骨Ca、着色料（カラメル、フラボノイド、クチナシ、紅麹）、香料、光沢剤、（一部にゼラチンを含む）</t>
-  </si>
-  <si>
-    <t>砂糖(タイ製造、国内製造)、牛乳、全粉乳、メロン果汁、脱脂粉乳、ココナッツオイル、デキストリン、クリーム、食塩／乳化剤、香料、ビタミンC、クチナシ色素、カロテン色素、甘味料(ステビア)、クエン酸</t>
-  </si>
-  <si>
     <t>小麦粉（国内製造）、砂糖、カカオマス、全粉乳、植物油脂、ショートニング、マーガリン（乳成分を含む）、乳糖、バター、ココアバター、脱脂粉乳、加糖練乳、液全卵、うるちひえパフ、ごま、ぶどう糖、食塩、乾燥卵白（卵を含む）／リン酸Ca、乳化剤（大豆由来）、膨脹剤、香料（乳由来）、着色料（カロテノイド）、ビタミンＤ</t>
   </si>
   <si>
-    <t>小麦粉（国内製造）、砂糖、全粉乳、ショートニング、ココアバター、マーガリ（乳成分を含む）、液全卵、イースト、食用加工油脂（小麦を含む）、カラメル粉末（乳成分を含む）、乳糖、キャラメル粉末（乳成分を含む）、洋酒、うるちひえパフ、食塩、液卵白(卵を含む)、カカオマス、水飴／ソルビトール、卵殻未焼成カルシウム（卵由来）、酒精、乳化剤（大豆由来）、香料（乳由来）、イーストフード（小麦由来）、トレハロース、ビタミンＣ、ビタミンＤ、着色料（カロテン）</t>
-  </si>
-  <si>
-    <t>チョコレート（砂糖、全粉乳、植物油脂、ココアバター、カカオマス、乳糖）、ウエハース（小麦粉、澱粉、砂糖、植物油脂、ミルクカルシウム、食塩）／乳化剤、香料、カラメル色素、膨脹剤、（一部に乳成分・小麦を含む）</t>
-  </si>
-  <si>
-    <t>ビスケット（小麦粉、砂糖、ショートニング、植物油脂、その他）（国内製造）、準チョコレート（砂糖、植物油脂、ココアパウダー、全粉乳、脱脂粉乳、その他）／乳化剤、香料、カラメル色素、膨脹剤、（一部に卵・乳成分・小麦を含む）</t>
-  </si>
-  <si>
-    <t>ピーナッツ（中国）、澱粉、米（国産）、しょう油、植物油脂、砂糖、デキストリン、食塩、かつおエキス、香辛料／加工でん粉、調味料（アミノ酸等）、着色料（カラメル、カロチノイド、紅麹）、香辛料抽出物、（一部に小麦・落花生・大豆を含む）</t>
-  </si>
-  <si>
-    <t>植物油脂（国内製造）、砂糖、ショートニング、ポテトでん粉、青大豆、枝豆パウダー（秋田県産）、チーズ、マルチトール、乾燥ポテト、食塩、バター、クロレラパウダー、香辛料、たん白加水分解物、酵母エキスパウダー、大豆イソフラボン抽出物、デキストリン／加工でん粉、カゼインNa、乳化剤、膨脹剤、炭酸Ca、香料、調味料（アミノ酸）、（一部に小麦・乳成分・大豆・ゼラチンを含む）</t>
-  </si>
-  <si>
-    <t>小麦粉、砂糖、植物油脂、カカオマス、ショートニング、ココアパウダー、全粉乳、転化糖蜜、加糖れん乳、ごま、食塩、コラーゲン(豚肉を含む)／着色料（カラメル）、膨脹剤、乳化剤（大豆由来）、炭酸Ｃａ、香料</t>
-  </si>
-  <si>
-    <t>ポテトフレーク（外国製造）、植物油脂、砂糖、フライドポテト風味パウダー、食塩、味付けフリーズドライポテトダイス、こんぶエキス、たんぱく加水分解物、全卵粉末／加工デンプン、乳化剤、酸化防止剤(ビタミンE、ビタミンC）、調味料（アミノ酸等）、香料、糊料（加工デンプン）、（一部に小麦・卵・ごま・大豆・鶏肉・豚肉を含む）</t>
-  </si>
-  <si>
-    <t>小麦粉(国内製造)、植物油脂、えび粉末、えび塩風味パウダー、食塩、ローストしょうゆパウダー／加工デンプン、炭酸Ca、調味料（アミノ酸等）、酸化防止剤（ビタミンＥ、ビタミンC）、乳化剤、香料、カラメル色素、（一部にえび・小麦・大豆・鶏肉・豚肉を含む）</t>
-  </si>
-  <si>
-    <t>コーン(遺伝子組換えでない)(米国産)、植物油、砂糖、粉末醤油、ぶどう糖、食塩、オニオンパウダー、香辛料、ポークエキスパウダー、酵母エキスパウダー／調味料(アミノ酸等)、香料、着色料(カラメル、カロチノイド)、甘味料(アセスルファムK、ステビア、カンゾウ)、酸味料、(一部に小麦・ごま・大豆・豚肉を含む)</t>
-  </si>
-  <si>
     <t>ぶどう糖、砂糖、水あめ、還元水あめ/ガムベース、酸味料、香料、軟化剤、着色料（カラメル、フラボノイド）</t>
   </si>
   <si>
-    <t>じゃがいも（国産）、植物油、乾燥じゃがいも、ミルクパウダー、粉末植物油脂、砂糖、粉末しょうゆ（小麦・大豆を含む）、食塩、乳糖、でん粉、デキストリン、酵母エキスパウダー、たん白加水分解物、焼きのり、酒粕パウダー、チキンエキスパウダー、混合節エキスパウダー（さばを含む）、わさびパウダー / 調味料（アミノ酸等）、香料、加工デンプン、乳化剤、酸味料、カラメル色素、酸化防止剤（Ｖ．Ｃ）</t>
-  </si>
-  <si>
     <t>ぶどう糖、砂糖、でん粉、ゼラチン、酸味料、乳化剤、光沢剤、香料、着色料（クチナシ、野菜色素、カロチノイド）、糊料（アラビアガム）</t>
   </si>
   <si>
-    <t>植物油脂、砂糖、コーン（遺伝子組み換えでない）、全粉乳、ココア、カカオマス、パン粉、脱脂粉乳、食塩、乳化剤（大豆由来）、香料、（原材料の一部に小麦を含む）</t>
-  </si>
-  <si>
     <t>小麦粉（国内製造）、植物油脂、ソース(砂糖、野菜・果実、醸造酢、食塩、アミノ酸液、その他)、砂糖、食塩、ソース風味パウダー、香辛料、アオサ粉、野菜パウダー、ミート調味エキス、野菜エキス、魚介エキス、魚醤パウダー（魚介類）／加工デンプン、調味料(アミノ酸等)、炭酸Ca、香料、カラメル色素、乳化剤、酸味料、酸化防止剤(ビタミンE)、香辛料抽出物、（一部に小麦・卵・乳成分・魚醤パウダー（魚介類）・牛肉・さば・大豆・鶏肉・豚肉・もも・りんごを含む）</t>
   </si>
   <si>
-    <t>砂糖混合ぶどう糖果糖液糖、酸味料、香料、着色料(黄色4号）</t>
-  </si>
-  <si>
-    <t>果糖ぶどう糖液糖、食塩／炭酸、酸味料、香料</t>
-  </si>
-  <si>
-    <t>果糖ぶどう糖液糖、梨果汁(広島県産)、酸味料、香料</t>
-  </si>
-  <si>
-    <t>果糖ぶどう糖液糖、桃果汁（岡山県産）、酸味料、香料</t>
-  </si>
-  <si>
-    <t>果糖ぶどう糖液糖、マスカット果汁（岡山県産）、酸味料、香料</t>
-  </si>
-  <si>
-    <t>果糖ぶどう糖液糖、レモン果汁(広島県産)、酸味料、香料</t>
-  </si>
-  <si>
-    <t>果糖ぶどう糖液糖、はっさく果汁(広島県産)、酸味料、香料</t>
-  </si>
-  <si>
-    <t>果糖ぶどう糖液糖/炭酸、酸味料</t>
-  </si>
-  <si>
     <t>果糖ぶどう糖液糖（国内製造）/炭酸、酸味料、香料</t>
   </si>
   <si>
-    <t>砂糖(国内製造)、ぶどう糖、水飴、でん粉/ガムベース、軟化剤、酸味料、香料、着色料（紅花黄、クチナシ)</t>
-  </si>
-  <si>
     <t>砂糖（国内製造）、ぶどう糖、水飴、でん粉、ピーチ果汁／ガムベース、酸味料、軟化剤、香料、着色料（カラメル、アントシアニン、紅花黄、クチナシ）</t>
   </si>
   <si>
-    <t>砂糖（タイ製造）、水あめ、ゼラチン、食用油脂／甘味料（ソルビトール）、酸味料、ゲル化剤（ペクチン：オレンジ由来）、着色料（カラメル）、香料</t>
-  </si>
-  <si>
-    <t>砂糖（タイ製造）、水あめ、ゼラチン、グレープ濃縮果汁、食用油脂／甘味料（ソルビトール）、酸味料、ゲル化剤（ペクチン：オレンジ由来）、香料、着色料（野菜色素、クチナシ）</t>
-  </si>
-  <si>
-    <t>砂糖（タイ製造）、水あめ、ゼラチン、りんご濃縮果汁、食用油脂／甘味料（ソルビトール）、酸味料、ゲル化剤（ペクチン：オレンジ由来）、香料、着色料（クチナシ）</t>
-  </si>
-  <si>
-    <t>えんどう豆（輸入）、でん粉、食用油脂、砂糖、小麦粉、水あめ、食塩、ぶどう糖、配合調味料、わさび葉パウダー／香料、調味料（アミノ酸等）、膨脹剤、環状オリゴ糖、乳化剤、着色料（黄4、青1）、（一部に小麦・大豆を含む）</t>
-  </si>
-  <si>
-    <t>油揚げめん（小麦粉（国内製造）、植物油脂、食塩、しょうゆ、香辛料、大豆食物繊維）、ソース（豚脂、みそ、糖類、甜麺醤、還元水あめ、食塩、ポークエキス、香辛料、粉末みそ、たん白加水分解物、オニオンエキス）、かやく（キャベツ、大豆たん白加工品、にんじん）／加工でん粉、カラメル色素、調味料（アミノ酸等）、増粘剤（加工でん粉、アラビアガム）、酒精、炭酸Ｃａ、かんすい、酸味料、香料、グリセリン、フラボノイド色素、クチナシ色素、酸化防止剤（ビタミンＥ）、ｐＨ調整剤、乳化剤、甘味料（スクラロース、アセスルファムＫ）、炭酸Ｍｇ、ビタミンＢ２、ビタミンＢ１、（一部に小麦・卵・乳成分・ごま・大豆・豚肉を含む）</t>
-  </si>
-  <si>
-    <t>油揚げめん（小麦粉（国内製造）、そば粉、植物油脂、食塩、植物性たん白、しょうゆ）、スープ（糖類、食塩、かつおぶし調味料、粉末しょうゆ、魚粉（かつお、そうだかつお、いわし）、オニオン調味料、ねぎ、たん白加水分解物、デキストリン、香辛料）、かやく（揚げ玉、味付卵、かまぼこ、わかめ）／加工でん粉、調味料（アミノ酸等）、リン酸塩（Ｎａ）、カラメル色素、炭酸Ｃａ、香料、酸味料、酸化防止剤（ビタミンＥ）、乳化剤、増粘多糖類、ベニコウジ色素、チャ抽出物、カロテン色素、ビタミンＢ２、クチナシ色素、ビタミンＢ１、（一部にえび・小麦・そば・卵・乳成分・さば・大豆・鶏肉・豚肉を含む）</t>
-  </si>
-  <si>
-    <t>油揚げめん（小麦粉（国内製造）、植物油脂、食塩、大豆食物繊維、デキストリン)、スープ（食塩、粉末しょうゆ、かつおぶし調味料、魚粉（かつお、さば、いわし）、にぼし調味料、ねぎ、こんぶ粉末、糖類、香辛料）、かやく（味付油揚げ、味付卵、かまぼこ、わかめ）／加工でん粉、調味料（アミノ酸等）、リン酸塩（Ｎａ）、炭酸Ｃａ、増粘多糖類、乳化剤、香料、ｐＨ調整剤、カラメル色素、酸化防止剤（ビタミンＥ）、微粒二酸化ケイ素、パプリカ色素、クチナシ色素、チャ抽出物、カロテン色素、ビタミンＢ２、ビタミンＢ１、ベニコウジ色素、（一部に小麦・卵・乳成分・さば・大豆・鶏肉・豚肉・ゼラチンを含む）</t>
-  </si>
-  <si>
-    <t>油揚げめん（小麦粉（国内製造）、植物油脂、食塩、大豆食物繊維、デキストリン）、スープ（糖類、食塩、粉末しょうゆ、香味調味料、にぼし調味料、ビーフ調味料、魚粉（かつお、そうだかつお）、香辛料、たん白加水分解物）、かやく（大豆たん白加工品、揚げ玉、わかめ、ねぎ）／加工でん粉、調味料（アミノ酸等）、リン酸塩（Ｎａ）、炭酸Ｃａ、増粘剤（アラビアガム）、カラメル色素、香料、乳化剤、酸味料、香辛料抽出物、微粒二酸化ケイ素、ｐＨ調整剤、酸化防止剤（ビタミンＥ）、チャ抽出物、ビタミンＢ２、ビタミンＢ１、ベニコウジ色素、（一部にえび・小麦・卵・乳成分・牛肉・ごま・大豆・鶏肉・豚肉・ゼラチンを含む）</t>
-  </si>
-  <si>
-    <t>油揚げめん（小麦粉（国内製造）、植物油脂、食塩、大豆食物繊維、デキストリン）、スープ（食塩、ポーク調味料、糖類、魚醤、ごま、クリーミングパウダー、たん白加水分解物、香辛料、粉末みそ、香味調味料、あさり調味料）、かやく（卵、赤唐辛子、わかめ、ねぎ）／加工でん粉、調味料（アミノ酸等）、香料、リン酸塩（Ｎａ）、増粘多糖類、炭酸Ｃａ、乳化剤、カラメル色素、酸味料、微粒二酸化ケイ素、カロチノイド色素、ｐＨ調整剤、香辛料抽出物、酸化防止剤（ビタミンＥ）、ビタミンＢ２、ビタミンＢ１、（一部に小麦・卵・乳成分・ごま・大豆・豚肉・ゼラチンを含む）</t>
-  </si>
-  <si>
-    <t>じゃがいも（遺伝子組換えでない）（国産）、植物油脂、砂糖、たん白加水分解物（大豆を含む）、粉末しょうゆ（小麦を含む）、食塩、ビーフパウダー（鶏肉・ゼラチンを含む）、粉末ソース、酵母エキスパウダー、ガーリックパウダー、レッドペッパー、オニオンパウダー、デキストリン、ぶどう糖、わさびパウダー/調味料（アミノ酸等）、香料、甘味料（ステビア、スクラロース）、酸味料、カゼインナトリウム（乳由来）、カラメル色素、香辛料抽出物</t>
-  </si>
-  <si>
-    <t>じゃがいも（遺伝子組換えでない）（国産）、植物油脂、砂糖、食塩、粉末しょうゆ（小麦・大豆を含む）、粉末油脂、酵母エキスパウダー、香辛料、調味油、たん白加水分解物、乳糖、バター／調味料（アミノ酸等）、香料（ごま由来）、甘味料（ステビア）、酸味料</t>
-  </si>
-  <si>
-    <t>じゃがいも（遺伝子組換えでない）（国産）、植物油脂、砂糖、食塩、オニオンパウダー、オニオンエキスパウダー、たん白加水分解物（大豆・豚肉を含む）、酵母エキスパウダー、パセリ、オリゴ糖、サワークリームパウダー（北海道産サワークリーム使用）、乳糖／調味料（アミノ酸等）、酸味料、香料、甘味料（スクラロース、ステビア、カンゾウ）</t>
-  </si>
-  <si>
-    <t>じゃがいも（遺伝子組換えでない）（国産）、植物油脂、砂糖、香辛料、たん白加水分解物（大豆・豚肉を含む）、粉末しょうゆ（小麦を含む）、食塩、マヨネーズ風味パウダー（卵を含む）、乳等を主要原料とする食品、オリゴ糖、デキストリン、明太子パウダー（ゼラチンを含む）、ビーフパウダー（鶏肉を含む）／調味料（アミノ酸等）、香料、酸味料、カロチノイド色素、甘味料（ステビア、スクラロース）、香辛料抽出物、ウコン色素</t>
-  </si>
-  <si>
-    <t>じゃがいも（遺伝子組換えでない）（国産）、植物油脂、砂糖、たん白加水分解物（大豆を含む）、粉末しょうゆ（小麦を含む）、ビーフパウダー（鶏肉・ゼラチンを含む）、食塩、ガーリックパウダー、デキストリン、わさびパウダー／調味料（アミノ酸等）、香料、甘味料（ステビア、スクラロース）、カゼインナトリウム（乳由来）、香辛料抽出物、酸味料</t>
-  </si>
-  <si>
-    <t>ぶどう糖（国内製造）、乳糖（乳成分を含む）、砂糖／酸味料、重曹、乳化剤、香料、着色料（カラメル、麦芽エキス）、甘味料（アセスルファムK）</t>
-  </si>
-  <si>
-    <t>果糖ブドウ糖液糖（国内製造）、砂糖、濃縮りんご果汁、寒天／甘味料（ソルビトール）、ゲル化剤（増粘多糖類）、酸味料、香料、乳酸カルシウム、乳化剤、着色料（野菜色素、クチナシ、紅花黄）</t>
-  </si>
-  <si>
-    <t>砂糖（国内製造、外国製造）、小麦粉、植物油脂、乳糖、でん粉、ショートニング、ココアバター、全粉乳、ホエイパウダー、液卵、乳等を主要原料とする食品（はっ酵バター、植物油脂、バターオイル、脱脂粉乳、食塩）、脱脂粉乳、クリームパウダー、食塩、レモンピールパウダー／膨脹剤、酸味料、着色料（カラメル、クチナシ）、乳化剤（大豆由来）、香料</t>
-  </si>
-  <si>
     <t>＜れもん＞水あめ（国内製造）、砂糖、ゼラチン、濃縮レモン果汁、オブラートパウダー／ソルビトール、グリセリン、酸味料、ゲル化剤（ペクチン）、香料、乳化剤、紅花色素、光沢剤＜コーラ＞水あめ（国内製造）、砂糖、ゼラチン、コーラナッツエキス、オブラートパウダー／ソルビトール、グリセリン、酸味料、ゲル化剤（ペクチン）、カラメル色素、香料、乳化剤、光沢剤＜ソーダ＞水あめ（国内製造）、砂糖、ゼラチン、オブラートパウダー／ソルビトール、グリセリン、酸味料、ゲル化剤（ペクチン）、香料、クチナシ色素、乳化剤、光沢剤＜ぶどう＞水あめ（国内製造）、砂糖、ゼラチン、濃縮グレープ果汁、オブラートパウダー／ソルビトール、グリセリン、酸味料、ゲル化剤（ペクチン）、香料、着色料（ブラックキャロットジュース、クチナシ）、乳化剤、光沢剤</t>
   </si>
   <si>
-    <t>油揚げめん（小麦粉（国内製造）、植物油脂、ラード、しょうゆ、食塩、たん白加水分解物、チキンエキス、ポークエキス、野菜エキス）、スープ（しょうゆ、食塩、動物油脂、植物油脂、糖類、みそ、たん白加水分解物、チキンエキス、ポークエキス、鰹エキス）、かやく（味付肉そぼろ、ねぎ、赤ピーマン）／加工でん粉、調味料（アミノ酸等）、増粘剤（加工でん粉、増粘多糖類）、カラメル色素、かんすい、香料、酸化防止剤（ビタミンE、ローズマリー抽出物）、カロチノイド色素、香辛料抽出物、酸味料、（一部に卵・小麦・ごま・大豆・鶏肉・豚肉を含む）</t>
-  </si>
-  <si>
-    <t>油揚げめん（小麦粉（国内製造）、植物油脂、ラード、しょうゆ、食塩、たん白加水分解物、チキンエキス、ポークエキス、野菜エキス）、スープ（しょうゆ、食塩、糖類、動物油脂、デキストリン、野菜粉末、植物油脂、香辛料、ポークエキス、でん粉、チキンエキス、オイスターエキス）、かやく（モヤシ、ニンジン、ニラ）／加工でん粉、調味料（アミノ酸等）、増粘多糖類、カラメル色素、酒精、香料、かんすい、酸化防止剤（ビタミンE)、クチナシ色素、（一部に乳成分・小麦・ごま・大豆・鶏肉・豚肉を含む）</t>
-  </si>
-  <si>
-    <t>油揚げめん（小麦粉（国内製造）、植物油脂、ラード、しょうゆ、食塩、たん白加水分解物、チキンエキス、ポークエキス、野菜エキス）、スープ（しょうゆ、食塩、糖類、動物油脂、たん白加水分解物、香辛料、ポークエキス）、かやく（味付豚肉、ねぎ）／加工でん粉、調味料（アミノ酸等）、酒精、カラメル色素、増粘多糖類、かんすい、酸化防止剤（ビタミンE)、香辛料抽出物、クチナシ色素、（一部に小麦・大豆・鶏肉・豚肉を含む）</t>
-  </si>
-  <si>
-    <t>油揚げめん（小麦粉（国内製造）、植物油脂、ラード、しょうゆ、食塩、たん白加水分解物、チキンエキス、ポークエキス、野菜エキス）、スープ（食塩、糖類、動物油脂、香辛料、たん白加水分解物、魚醤パウダー（魚介類）、しょうゆ、ポークエキス、酵母エキス、みそ、キムチパウダー、オニオンパウダー、植物油脂）、かやく（白菜キムチ、フライドガーリック、ニラ）／加工でん粉、調味料（アミノ酸等）、増粘多糖類、カラメル色素、かんすい、カロチノイド色素、酸化防止剤（ビタミンE、ビタミンC）、微粒二酸化ケイ素、酸味料、香料、（一部に乳成分・小麦・ごま・大豆・鶏肉・豚肉・魚醤パウダー（魚介類）を含む）</t>
-  </si>
-  <si>
-    <t>油揚げめん（小麦粉（国内製造）、植物油脂、ラード、しょうゆ、食塩、たん白加水分解物、チキンエキス、ポークエキス、野菜エキス）、スープ（しょうゆ、ポークエキス、動物油脂、たん白加水分解物、食塩、糖類、ニンニクペースト、酵母パウダー、食用風味油、香辛料）、かやく（味付豚肉、焼のり、ねぎ）／加工でん粉、調味料（アミノ酸等）、酒精、カラメル色素、増粘多糖類、かんすい、酸化防止剤（ビタミンE）、クチナシ色素、香辛料抽出物、（一部に小麦・大豆・鶏肉・豚肉を含む）</t>
-  </si>
-  <si>
-    <t>馬鈴薯（国産）（遺伝子組換えでない）、植物油脂、岩塩シーズニング（ぶどう糖、食塩（フランス産岩塩９０％）、砂糖、チキンブイヨンパウダー、粉末油脂、香辛料、マッシュルームエキスパウダー、たん白加水分解物、ホタテエキスパウダー、昆布エキスパウダー、酵母エキスパウダー）／調味料（アミノ酸等）、香料、酸味料、甘味料（スクラロース）、（一部に小麦・乳成分・大豆・鶏肉・豚肉を含む）</t>
-  </si>
-  <si>
-    <t>原材料名：油揚げめん（小麦粉（国内製造）、植物油脂、ラード、しょうゆ、食塩、香辛料）、添付調味料（糖類、たん白加水分解物、食塩、しょうゆ、醸造酢、植物油脂、りんごピューレ、香辛料、トマトペースト、ポークエキス、野菜エキス）、かやく（キャベツ、唐辛子）/調味料（アミノ酸等）、香辛料抽出物、酒精、カラメル色素、増粘多糖類、かんすい、パプリカ色素、酸化防止剤（ビタミンE）、甘味料（ステビア）、ビタミンB2、（一部に小麦・大豆・豚肉・りんごを含む）</t>
-  </si>
-  <si>
-    <t>うるち米（国内産）、植物油脂、しょうゆ（小麦、大豆を含む）、砂糖、かつおだし粉末、昆布だし/加工デンプン、調味料（アミノ酸等）、貝カルシウム</t>
-  </si>
-  <si>
-    <t>準チョコレート（砂糖、植物油脂（大豆を含む）、全粉乳、乳糖、カカオマス、ココアパウダー）（国内製造）、小麦粉、鶏卵、砂糖、デキストリン、ショートニング、食塩／乳化剤（大豆由来）、膨脹剤、香料</t>
-  </si>
-  <si>
-    <t>砂糖（外国製造、国内製造）、カカオマス、乳糖、植物油脂（大豆を含む）、全粉乳、デキストリン、水あめ／加工でん粉、卵殻Ｃａ、光沢剤、乳化剤（大豆由来）、着色料（赤ビート、クチナシ、カラメル、カロテン、紅花黄、フラボノイド）、増粘剤（アラビアガム）、香料</t>
-  </si>
-  <si>
-    <t>糖類（異性化液糖、砂糖、果糖）（国内製造）、グレープ濃縮果汁／ゲル化剤（増粘多糖類）、酸味料、香料、着色料（アントシアニン）、酸化防止剤（ビタミンC、酵素処理ルチン）</t>
-  </si>
-  <si>
-    <t>準チョコレート（砂糖、乳糖、植物油脂、全粉乳、ココアバター）（国内製造）、小麦粉、植物油脂、乳糖、砂糖、紅茶エキスパウダー、イースト、ココアパウダー、全粉乳、カカオマス、ココアバター／乳化剤、カラメル色素、香料、重曹、イーストフード、（一部に小麦・乳成分・大豆を含む）</t>
-  </si>
-  <si>
-    <t>ポテトペレット（じゃがいもでん粉、乾燥じゃがいも、その他）（スペイン産）、植物油、デキストリン、ぶどう糖、たん白加水分解物、食塩、昆布エキスパウダー、でん粉、酵母エキスパウダー、チキンエキスパウダー、オニオンパウダー、香料油/調味料（アミノ酸等）、香料、酸味料、香辛料抽出、（一部に小麦・牛肉・大豆・鶏肉・豚肉を含む）</t>
-  </si>
-  <si>
-    <t>ポテトペレット（じゃがいもでん粉、乾燥じゃがいも、その他）（スペイン製造）、植物油、砂糖、オニオンパウダー、ローストオニオンパウダー、食塩、コーンスターチ、ビーフエキスパウダー、酵母エキスパウダー、白菜エキスパウダー、たん白加水分解物、ミルポワパウダー、こしょうパウダー、セロリ/調味料（アミノ酸等）、香料、甘味料（アスパルテーム・L-フェニルアラニン化合物、ステビア）、パプリカ色素、（一部に小麦・牛肉・大豆・鶏肉・豚肉を含む）</t>
-  </si>
-  <si>
-    <t>ひよこ豆ペレット（ひよこ豆粉、じゃがいもでん粉、乾燥じゃがいも、その他）（スペイン製造）、植物油、大豆たんぱく、砂糖、酵母エキスパウダー、食塩、オニオンパウダー、ぶどう糖、ガーリックパウダー、サワークリームパウダー、ライムジュースパウダー、パセリフレーク、粉末油/調味料（アミノ酸等）、香料、酸味料、甘味料（ステビア）、（一部に小麦・乳成分・大豆）</t>
-  </si>
-  <si>
-    <t>ひよこ豆ペレット（ひよこ豆粉、じゃがいもでん粉、乾燥じゃがいも、その他）（スペイン製造）、パーム湯、大豆たんぱく、デキストリン、食塩、ぶどう糖、黒コショウパウダー、たん白加水分解物、チキンエキスパウダー、酵母エキスパウダー、ガーリックパウダー、オリーブオイル、粉末醤油/調味料（アミノ酸等）、香料、（一部に小麦・大豆・鶏肉を含む）</t>
-  </si>
-  <si>
-    <t>水あめ（国内製造）、還元水あめ/ソルビトール、酸味料、増粘剤（プルラン）、着色料（アントシアニン、クチナシ、カロチノイド）、香料</t>
-  </si>
-  <si>
-    <t>水あめ（国内製造）、ゼラチン、パラチニット/酸味料、香料、甘味料（スクラロース）、カロチノイド色素、ナイアシン</t>
-  </si>
-  <si>
-    <t>砂糖(国内製造）、砂糖調製品（砂糖、コーンスターチ）、ばれいしょでん粉、コーンスターチ、デキストリン/酸味料（クエン酸）、香料、アナトー色素、ブドウ果汁色素</t>
-  </si>
-  <si>
-    <t>砂糖、水飴、白桃果汁パウダー/乳化剤、酸味料、香料、果実色素</t>
-  </si>
-  <si>
-    <t>小麦粉（国内製造）、チョコレートチップ、ショートニング、砂糖、でん粉、鶏卵、ココアパウダー、食塩、スパイス／膨張剤、乳化剤、香料、カロテン色素、（一部に小麦・卵・乳成分・大豆を含む）</t>
-  </si>
-  <si>
-    <t>馬鈴薯（日本：遺伝子組換えでない）、植物油、砂糖、ぶどう糖、たんぱく加水分解物（大豆を含む）、香辛料（大豆を含む）、食塩、ミートエキス調味パウダー（乳成分・小麦・牛肉・ごま・大豆・鶏肉・豚肉を含む）、オリゴ糖、酵母エキスパウダー、香味油（小麦・大豆を含む）／調味料（アミノ酸等）、酸味料、パプリカ色素、香辛料抽出物、甘味料（アスパルテーム・Ｌ－フェニルアラニン化合物）、香料（小麦・大豆由来）</t>
-  </si>
-  <si>
-    <t>馬鈴薯（日本：遺伝子組換えでない）、植物油、砂糖、食塩、香辛料（大豆を含む）、ぶどう糖、ミートエキス調味パウダー（乳成分・小麦・ごま・大豆・鶏肉・豚肉を含む）、たんぱく加水分解物（大豆を含む）、酵母エキスパウダー、オリゴ糖、香味油（小麦・大豆を含む）、りんご果汁パウダー／調味料（アミノ酸等）、酸味料、パプリカ色素、甘味料（スクラロース、ステビア、カンゾウ）、香料、香辛料抽出物</t>
-  </si>
-  <si>
-    <t>馬鈴薯（日本：遺伝子組換えでない）、植物油、ガーリックパウダー、ぶどう糖、食塩、砂糖、たんぱく加水分解物（大豆を含む）、野菜エキスパウダー（乳成分・大豆・豚肉・ゼラチンを含む）、オニオン、ホワイトペパー、唐辛子／調味料（アミノ酸等）、香辛料抽出物、甘味料（ステビア、カンゾウ）、香料、カラメル色素、酸味料</t>
-  </si>
-  <si>
-    <t>馬鈴薯（日本：遺伝子組換えでない）、植物油、砂糖、ぶどう糖、岩塩、チーズパウダー（乳成分を含む）、クリーミングパウダー（乳成分を含む）、粉末発酵乳、粉末油脂（乳成分を含む）、たんぱく加水分解物（小麦を含む）、乳等を主要原料とする食品、オリゴ糖、香味油（小麦・大豆を含む）／調味料（アミノ酸）、酸味料、香料（乳・小麦・大豆由来）、パプリカ色素、香辛料抽出物</t>
-  </si>
-  <si>
-    <t>とうもろこし（アメリカ：遺伝子組換えの混入を防ぐため分別）、植物油、デキストリン、ぶどう糖、食塩、たんぱく加水分解物（鶏肉を含む）、チーズパウダー（乳成分を含む）、香辛料、乳等を主要原料とする食品、アンチョビパウダー（魚醤（魚介類）を含む）、酒粕パウダー、粉末しょうゆ（小麦・大豆を含む）、トリュフ／調味料（アミノ酸）、香料、カラメル色素、酸味料、カロチノイド色素</t>
-  </si>
-  <si>
-    <t>乾燥ポテト（外国製造）、植物油脂、澱粉、砂糖、ラード、ポテト風味シーズニング（食塩、砂糖、デキストリン、ポテトパウダー、たんぱく加水分解物加工品、たんぱく加水分解物、チキン風味パウダー、昆布エキスパウダー）、食塩、小麦粉／加工澱粉、調味料（アミノ酸等）、乳化剤、香料、酸味料、（一部に乳成分・小麦・牛肉・大豆・鶏肉・ゼラチンを含む）</t>
-  </si>
-  <si>
-    <t>乾燥ポテト（外国製造）、植物油脂、澱粉、砂糖、ラード、コンソメ風味シーズニング（オニオンパウダー、ブドウ糖、食塩、チキンエキスパウダー、粉末醤油、ミルポアパウダー、粉末ソース、香辛料、酵母エキスパウダー）、食塩、小麦粉／加工澱粉、調味料（アミノ酸等）、乳化剤、香料、甘味料（ステビア）、炭酸Ca、酸味料、カラメル色素、（一部に乳成分・小麦・牛肉・大豆・鶏肉を含む）</t>
-  </si>
-  <si>
-    <t>乾燥ポテト（外国製造）、植物油脂、落花生、唐辛子パウダー、食塩、ガーリックパウダー、砂糖、オニオンパウダー、酵母エキスパウダー、たんぱく加水分解物、ブドウ糖、澱粉、チリパウダー、乳糖、チキンパウダー、ホワイトペッパーパウダー、クミンパウダー、醤油風味調味料、チキンエキス調味料、パプリカパウダー、ハバネロピューレ、調味エキス／加工澱粉、調味料（アミノ酸等）、炭酸Ca、香料、酸化防止剤（ビタミンE）、酸味料、香辛料抽出物、カラメル色素、（一部に乳成分・小麦・落花生・ごま・大豆・鶏肉・豚肉・ゼラチンを含む）</t>
-  </si>
-  <si>
     <t>コーングリッツ（国内製造）、砂糖、植物油脂、マーガリン、加糖れん乳、食塩、ハチミツ、バター／ソルビトール、未焼成Ca、香料、乳化剤、甘味料（アドバンテーム）、カロチノイド色素、（一部に乳成分・大豆を含む）</t>
   </si>
   <si>
-    <t>果糖ぶどう糖液糖(国内製造)、オレンジエキス／炭酸、酸味料、香料、ビタミンC、カロテン色素</t>
-  </si>
-  <si>
-    <t>果糖ぶどう糖液糖(国内製造)、グレープエキス／炭酸、酸味料、カラメル色素、香料、アントシアニン色素</t>
-  </si>
-  <si>
-    <t>果糖ぶどう糖液糖(国内製造)、メロンエキス／炭酸、酸味料、香料、ベニバナ色素、クチナシ色素</t>
-  </si>
-  <si>
-    <t>糖類(果糖ぶどう糖液糖(国内製造)、砂糖)／炭酸、香料、酸味料</t>
-  </si>
-  <si>
-    <t>＜ハローキティ＞ 砂糖(外国製造又は国内製造)、全粉乳、カカオマス、植物油脂、ココアバター、乳糖、脱脂粉乳、油脂加工品／乳化剤(大豆由来)、香料(乳・大豆由来)、野菜色素 ＜マイメロディ＞ 砂糖(外国製造又は国内製造)、全粉乳、カカオマス、植物油脂、ココアバター、乳糖、脱脂粉乳、油脂加工品／乳化剤(大豆由来)、香料(乳・大豆由来)、野菜色素 ＜ポチャッコ＞ 砂糖(外国製造又は国内製造)、全粉乳、カカオマス、植物油脂、ココアバター、乳糖、脱脂粉乳、油脂加工品／乳化剤(大豆由来)、香料(乳・大豆由来) ＜ポムポムプリン＞ 砂糖(外国製造又は国内製造)、全粉乳、カカオマス、植物油脂、ココアバター、乳糖、脱脂粉乳、油脂加工品／乳化剤(大豆由来)、香料(乳・大豆由来)、カロテノイド色素 ＜シナモロール＞ 砂糖(外国製造又は国内製造)、全粉乳、カカオマス、植物油脂、ココアバター、乳糖、脱脂粉乳、油脂加工品／乳化剤(大豆由来)、香料(乳・大豆由来)、野菜色素</t>
-  </si>
-  <si>
-    <t>砂糖（タイ製造）、水あめ、ゼラチン、濃縮いちご果汁、でん粉／ソルビット、酸味料、香料、着色料（アントシアニン、カロテノイド）、チャ抽出物、乳化剤（大豆由来）</t>
-  </si>
-  <si>
-    <t>チョコレート（砂糖、ココアバター、植物油脂、全粉乳、脱脂粉乳、乳糖、カカオマス）（国内製造）、小麦粉、砂糖、バター、カシューナッツ、準チョコレート（砂糖、植物油脂、全粉乳、脱脂粉乳、乳糖、カカオマス、ココアパウダー、食塩）、ココアクッキー、アーモンド、植物油脂、乳等を主要原料とする食品、ショートニング、バターオイル、ホエイパウダー、小麦全粒粉、食塩、コーンスターチ、ぶどう糖、脱脂粉乳、全粉乳／膨脹剤、乳化剤（大豆由来）、香料、甘味料（ソルビトール）</t>
-  </si>
-  <si>
     <t>うるち米粉（国産、タイ産）、植物油脂、砂糖、チーズ粉末、食塩、たまねぎ粉末、トマト粉末、にんにく粉末、酵母エキス粉末、バジル粉末、たんぱく加水分解物（大豆を含む）、チキンエキス粉末、唐辛子粉末、白こしょう粉末、大豆たんぱく、黒こしょう粉末、香味油(小麦・大豆を含む)／加工デンプン、調味料（アミノ酸等）、香料（乳・小麦・大豆・鶏肉由来）、乳化剤(大豆由来)、酸味料、酸化防止剤（ビタミンE）、着色料（カロテノイド）、微粒酸化ケイ素、香辛料抽出物、リン酸三カルシウム</t>
   </si>
   <si>
-    <t>小麦粉（国内製造）、ショートニング、砂糖、玄米、米粉、油脂加工食品（乳成分を含む）、液全卵、抹茶、食塩／膨脹剤、着色料(紅花黄、クチナシ)、乳化剤(大豆由来)、香料、カゼインナトリウム(乳由来)</t>
-  </si>
-  <si>
-    <t>小麦粉（国内製造）、砂糖、ショートニング、カカオマス、ココアパウダー、液全卵、マーガリン（乳成分を含む）、植物油脂、油脂加工食品（乳成分を含む）、乳糖、食塩、シナモン粉末／乳化剤（大豆由来）、膨脹剤、香料、カゼインナトリウム（乳由来）</t>
-  </si>
-  <si>
-    <t>小麦粉（国内製造）、砂糖、ショートニング、白あん（生あん、砂糖、還元水飴、寒天、食塩）、コーンスターチ、異性化液糖、カカオマス、ファットスプレッド (乳成分を含む)、マーガリン (乳成分・大豆を含む)、水飴、植物油脂、液全卵、乳糖、食塩／ソルビトール、加工デンプン、着色料（カラメル、アナトー）、乳化剤（大豆由来）、香料 (乳由来)、膨脹剤、増粘剤（カラギーナン）</t>
-  </si>
-  <si>
-    <t>小麦粉（国内製造）、砂糖、ショートニング、全粉乳、植物油脂、加糖練乳、ぶどう糖、いちご粉末、食塩、ココアバター／膨脹剤、酸味料、乳化剤（大豆由来）、香料、着色料（ビートレッド、カロテン）、卵殻未焼成カルシウム（卵由来）</t>
-  </si>
-  <si>
-    <t>小麦粉（国内製造）、ショートニング、砂糖、乳糖、デキストリン、チーズ粉末、食塩／膨脹剤、乳化剤（大豆由来）、香料（乳・大豆由来）、着色料（カロテン）</t>
-  </si>
-  <si>
-    <t>うるち米（国産、アメリカ産）、植物油脂、砂糖、しょうゆ（小麦・大豆を含む）、果糖ぶどう糖液糖、食塩、調味エキス（大豆を含む）／加工デンプン（小麦由来）、調味料（アミノ酸等）、着色料（カラメル）</t>
-  </si>
-  <si>
-    <t>うるち米粉（国産、タイ産）、植物油脂、粉末醸造酢、砂糖、食塩、酵母エキス粉末、香辛料（ごまを含む）、チキンエキス粉末、粉末しょうゆ（小麦・大豆を含む）、でん粉、デキストリン／加工デンプン、香料（鶏肉由来）、調味料（アミノ酸等）、酸味料、酸化防止剤（ビタミンＥ）、微粒酸化ケイ素、着色料（カロテン）、香辛料抽出物、ビタミンＢ１、乳化剤（大豆由来）</t>
-  </si>
-  <si>
-    <t>ピーナッツ（輸入）、小麦粉、砂糖、澱粉、しょう油、焼きとうもろこし風味シーズニング、寒梅粉、醸造調味料、デキストリン、砂糖混合異性化液糖、植物油脂、酵母エキス、食塩／調味料（アミノ酸等）、加工でん粉、膨張剤、香料、増粘剤（加工でん粉）、乳化剤、糊料（プルラン）、甘味料（スクラロース）、　　　　（一部に乳成分・小麦・落花生・大豆を含む）</t>
-  </si>
-  <si>
     <t>○ソーダ味：砂糖（国内製造）、水飴（国内製造）／酸味料、香料、着色料（クチナシ、紅花黄）○オレンジ味：砂糖（国内製造）、水飴（国内製造）／酸味料、香料、カロテノイド色素○グレープ味：砂糖（国内製造）、水飴（国内製造）、濃縮グレープ果汁／酸味料、香料、野菜色素、クチナシ色素○コーラ味：砂糖（国内製造）、水飴（国内製造）／酸味料、カラメル色素、香料</t>
   </si>
   <si>
@@ -475,40 +138,283 @@
     <t>砂糖類（砂糖（国内製造）、ぶどう糖）、高麗人参根エキス、Ｌ－カルニチンＬ－酒石酸塩、塩化Ｎａ、ガラナ種子エキス／炭酸、リン酸、クエン酸Ｎａ、カラメル色素、クエン酸、保存料（安息香酸Ｎａ）、香料、Ｌ－アルギニン、カフェイン、ナイアシン、甘味料（スクラロース）、イノシトール、　　　　　ビタミンＢ６、ビタミンＢ２、ビタミンＢ１２</t>
   </si>
   <si>
-    <t>砂糖類（砂糖、ぶどう糖）、高麗人参根エキス、Ｌ－カルニチンＬ－酒石酸塩、塩化Ｎａ、ガラナ種子エキス／クエン酸、炭酸、香料、クエン酸Ｎａ、甘味料（Ｄ－リボース、スクラロース）、Ｌ－アルギ二ン、保存料（安息香酸）、カフェイン、ナイアシン、着色料（アントシアニン）、イノシトール、ビタミンＢ６、ビタミンＢ２、ビタミンＢ１２</t>
-  </si>
-  <si>
-    <t>ぶどう糖（国内製造）、水あめ、でん粉／加工でん粉、乳化剤、カラメル色素、香料</t>
-  </si>
-  <si>
-    <t>砂糖、水飴、濃縮果汁（いちご、レモン、オレンジ、パインアップル、りんご、メロン、すもも）、酸味料、香料、着色料（紫コーン色素、パプリカ色素、カロチン、紅麹、クチナシ、紅花黄）</t>
-  </si>
-  <si>
-    <t>砂糖（外国製造、国内製造）、全粉乳、植物油脂、小麦粉、カカオマス、乳糖、ココアバター、バナナパウダー、キャラメルパウダー、ココアパウダー、イースト／乳化剤、香料、重曹、イーストフード、（一部に小麦・乳成分・大豆・バナナを含む）</t>
-  </si>
-  <si>
-    <t>糖類（果糖ぶどう糖液糖（国内製造）、砂糖）/ 炭酸、カラメル色素、酸味料、香料、カフェイン</t>
-  </si>
-  <si>
-    <t>砂糖（国内製造）、水あめ、菊花抽出物／香料、カフェイン、着色料（カカオ、クチナシ、カラメル）、ナイアシン、甘味料（アセスルファムＫ、スクラロース）、調味料（アミノ酸）、（一部にゼラチンを含む）</t>
-  </si>
-  <si>
-    <t>砂糖（国内製造、タイ製造）、小麦粉、ココアバター、液卵白（卵を含む）、ショートニング、植物油脂、全粉乳、乳糖、マーガリン、ホエイパウダー（乳成分を含む）、抹茶、水飴、食塩／乳化剤（大豆由来）、香料（乳由来）、着色料（カラメル）、膨脹剤</t>
-  </si>
-  <si>
-    <t>緑茶(国産）、ビタミンC</t>
-  </si>
-  <si>
-    <t>小麦粉（国内製造）、砂糖、乳糖、加工油脂、還元水あめ、卵、抹茶、植物油脂、マーガリン、脱脂粉乳、食塩、桜パウダー（デキストリン、桜ペースト（桜花塩漬、桜葉塩漬）、寒天、砂糖、桜エキス）、麦芽糖、小麦ファイバー、水あめ／乳化剤（大豆由来）、結晶セルロース、香料、着色料（クチナシ、アカビート、アナトー）、安定剤（加工デンプン）</t>
-  </si>
-  <si>
-    <t>砂糖（国内製造）、水飴、全粉乳、植物油脂、抹茶、食塩／香料、酸味料、乳化剤、（一部に乳成分・大豆を含む）</t>
-  </si>
-  <si>
-    <t>【バナナ味キャンディ】砂糖(国内製造)、水あめ、加工油脂、還元水あめ、ゼラチン、でん粉/ソルビトール、乳化剤、香料、酸味料、増粘剤(プルラン)、フラボノイド色素〈チョコクリーム〉チョコレート利用商品(国内製造)(砂糖、加工油脂、ココアパウダー、全粉乳、カカオマス)/乳化剤(大豆由来)、香料【カラフルトッピング】砂糖(国内製造)、でん粉/糊料(アラビアガム)、着色料(クチナシ、アントシアニン、カロチノイド)、酸味料</t>
-  </si>
-  <si>
-    <t>＜りんご味キャンディ＞砂糖、水あめ、加工油脂、還元水あめ、ゼラチン、でん粉／ソルビトール、酸味料、乳化剤、増粘剤（プルラン）、香料、着色料（アントシアニン、カロチノイド）＜りんご味水あめ＞水あめ／酸味料、アントシアニン色素、香料＜カラフルトッピング＞砂糖、でん粉／糊料（アラビアガム）、着色料（アントシアニン、クチナシ、カロチノイド）、酸味料</t>
+    <t>小麦粉（国内製造）、植物油脂、でん粉、スモークチーズパウダー、砂糖、小麦たんぱく、食塩、発酵調味料、こしょう、酵母エキス、デキストリン、麦芽糖／調味料（アミノ酸等）、香料、増粘剤（キサンタンガム）、乳化剤、着色料（アナトー色素）、酸味料、（一部に乳成分・小麦・大豆を含む）</t>
+  </si>
+  <si>
+    <t>小麦粉（国内製造）、植物油脂、でん粉、砂糖、小麦たんぱく、ポークエキス、オニオンペースト、食塩、しょうゆシーズニング、たんぱく加水分解物、にんにくパウダー、酵母エキス、こしょう、ベーコンエキス／調味料（アミノ酸等）、香料、乳化剤、増粘剤（キサンタンガム）、着色料（アナトー色素、カラメル）、酸味料、くん液、（一部に乳成分・小麦・大豆・豚肉を含む）</t>
+  </si>
+  <si>
+    <t>小麦粉、植物油脂、ショートニング、砂糖、食塩、イースト、果糖ぶどう糖液糖、モルトエキス、コンソメシーズニング、しょうゆシーズニング、調味料（無機塩等）、香料、（原材料の一部に乳成分、大豆、鶏肉を含む）</t>
+  </si>
+  <si>
+    <t>小麦粉（国内製造）、植物油脂、乾燥ポテト、でん粉、野菜エキスシーズニング、食塩、えだまめパウダー／トレハロース、調味料（アミノ酸等）、香料、乳化剤、クチナシ色素、酸味料、甘味料（スクラロース）、（一部に乳成分・小麦・大豆・ゼラチンを含む）</t>
+  </si>
+  <si>
+    <t>ぶどう糖（国内製造）、タピオカでん粉／酸味料、乳化剤、香料、アカキャベツ色素</t>
+  </si>
+  <si>
+    <t>水あめ、砂糖、植物油脂、ゼラチン、濃縮ストロベリー果汁、加糖練乳、ストロベリージャム、乳酸菌飲料、酸味料、乳化剤、香料、アカキャベツ色素</t>
+  </si>
+  <si>
+    <t>砂糖、水あめ、植物油脂、ラムネ菓子（エリスリトール、ポリデキストロース）、ゼラチン、デキストリン、濃縮レモン果汁、酸味料、乳化剤、香料、ステアリン酸カルシウム、ベニバナ黄色素</t>
+  </si>
+  <si>
+    <t>砂糖（国内製造、タイ製造）、水あめ、植物油脂、デキストリン、ゼラチン、濃縮りんご果汁／酸味料、グリセリン、香料、乳化剤、ベニバナ黄色素、クチナシ青色素</t>
+  </si>
+  <si>
+    <t>めん（小麦粉（国内製造）、食塩、植物油脂、植物性たん白、卵白）、添付調味料（しょうゆ、チキンエキス、食塩、植物油、鶏脂、ポークエキス、香辛料、砂糖、野菜エキス、発酵調味料、たん白加水分解物、酵母エキス、ミート風味パウダー、香味油脂）／加工でん粉、調味料（アミノ酸等）、トレハロース、かんすい、酒精、炭酸カルシウム、レシチン、酸化防止剤（ビタミンＣ、ビタミンＥ）、カラメル色素、クチナシ色素、増粘多糖類、香料、甘味料（カンゾウ）、香辛料抽出物、（一部に小麦・卵・乳成分・大豆・鶏肉・豚肉・ゼラチンを含む）</t>
+  </si>
+  <si>
+    <t>めん（小麦粉（国内製造）、食塩、植物性たん白、植物油脂、卵白）、添付調味料（ポークエキス、しょうゆ、鶏脂、食塩、でん粉、砂糖、香辛料、たん白加水分解物、野菜エキス、植物油）／加工でん粉、調味料（アミノ酸等）、トレハロース、かんすい、カラメル色素、炭酸カルシウム、増粘多糖類、酒精、レシチン、酸化防止剤（ビタミンＥ）、クチナシ色素、（一部に小麦・卵・乳成分・大豆・鶏肉・豚肉・ゼラチンを含む）</t>
+  </si>
+  <si>
+    <t>めん（小麦粉（国内製造）、植物油脂、食塩、植物性たん白、卵白）、添付調味料（しょうゆ、ラード、魚介エキス、食塩、チキンエキス、ポークエキス、香味油脂、砂糖、香辛料、酵母エキス）／加工でん粉、調味料（アミノ酸等）、トレハロース、かんすい、酒精、炭酸カルシウム、レシチン、酸化防止剤（ビタミンＣ、ビタミンＥ）、カラメル色素、クチナシ色素、増粘多糖類、香料、（一部に小麦・卵・さば・大豆・鶏肉・豚肉・ゼラチンを含む）</t>
+  </si>
+  <si>
+    <t>油揚げめん（小麦粉（国内製造）、植物油脂、精製ラード、食塩、植物性たん白）、添付調味料（食塩、香辛料、チキンエキス、しょうゆ、酵母エキス、砂糖、植物油）／加工でん粉、調味料（アミノ酸等）、炭酸カルシウム、カラメル色素、かんすい、酸化防止剤（ビタミンＥ）、酸味料、クチナシ色素、（一部に小麦・大豆・鶏肉・豚肉を含む）</t>
+  </si>
+  <si>
+    <t>油揚げめん（小麦粉（国内製造）、植物油脂、精製ラード、食塩）、添付調味料（食塩、しょうゆ、デキストリン、チキンエキス、ポークエキス、香辛料（黒こしょう、ガーリックパウダー））／加工でん粉、カラメル色素、炭酸カルシウム、調味料（アミノ酸等）、かんすい、酸化防止剤（ビタミンＥ）、クチナシ色素、香料、香辛料抽出物、（一部に小麦・卵・乳成分・ごま・大豆・鶏肉・豚肉を含む）</t>
+  </si>
+  <si>
+    <t>めん（小麦粉（国内製造）、食塩、植物性たん白、植物油脂、卵白）、添付調味料（みそ、ポークエキス、食塩、香辛料、香味油脂、野菜エキス、植物油、ラード、砂糖、発酵調味料、デーツ果汁、たん白加水分解物）／加工でん粉、調味料（アミノ酸等）、トレハロース、酒精、かんすい、炭酸カルシウム、カラメル色素、レシチン、酸化防止剤（ビタミンＥ）、クチナシ色素、（一部に小麦・卵・ごま・大豆・鶏肉・豚肉・ゼラチンを含む）</t>
+  </si>
+  <si>
+    <t>油揚げめん（小麦粉（国内製造）、植物油脂、食塩、ソース、糖類）、ソース（ソース、からしマヨネーズ、糖類、植物油脂、食塩、香味油、たん白加水分解物、ソース加工品、香味調味料、ポークエキス、香辛料、醸造酢）、かやく（キャベツ）、ふりかけ（ソース加工品、マヨネーズ風ソースフレーク、アオサ、紅しょうが）／カラメル色素、調味料（アミノ酸等）、炭酸カルシウム、かんすい、酸味料、乳化剤、香料、香辛料抽出物、酸化防止剤（ビタミンＥ）、炭酸マグネシウム、カロチノイド色素、ビタミンＢ２、ビタミンＢ１、（一部に卵･乳成分･小麦･えび･オレンジ･ごま･大豆･豚肉･りんごを含む）</t>
+  </si>
+  <si>
+    <t>油揚げめん（小麦粉（国内製造）、植物油脂、食塩、ホタテエキス、乳たん白）、スープ（食塩、ポークエキス、香辛料、たん白加水分解物、糖類、香味調味料、酵母エキス、しょうゆ、ローストオニオン粉末）／加工デンプン、調味料（アミノ酸等）、炭酸カルシウム、カラメル色素、かんすい、炭酸マグネシウム、増粘多糖類、香料、酸化防止剤（ビタミンＥ）、カロチノイド色素、酸味料、甘味料（スクラロース）、ビタミンＢ２、ビタミンＢ１、（一部に卵･乳成分･小麦･えび･ごま･大豆･鶏肉･豚肉を含む）</t>
+  </si>
+  <si>
+    <t>油揚げめん（小麦粉（国内製造）、植物油脂、食塩、卵粉、しょうゆ）、スープ（食塩、豚脂、ポークエキス、香辛料、香味油、たん白加水分解物、酵母エキス、しょうゆ、デキストリン、糖類、ローストオニオン粉末、香味調味料、植物油脂）、かやく（卵、豚・鶏味付肉、ニラ）/加工デンプン、調味料（アミノ酸等）、炭酸カルシウム、カラメル色素、かんすい、香料、増粘多糖類、ソルビット、グリセリン、カロチノイド色素、微粒二酸化ケイ素、乳化剤、酸化防止剤（ビタミンE）、酸味料、甘味料（スクラロース）、香辛料抽出物、ビタミンB2、ビタミンB1、（一部に卵・乳成分・小麦・ごま・大豆・鶏肉・豚肉を含む）</t>
+  </si>
+  <si>
+    <t>油揚げめん（小麦粉（国内製造）、植物油脂、食塩、しょうゆ）、スープ（食塩、ポークエキス、香辛料、トマトペースト、デキストリン、糖類、しょうゆ、たん白加水分解物、酵母エキス、ローストオニオン粉末、醸造酢、豚脂、香味調味料）、かやく（豚･鶏味付肉、卵、ニラ、赤唐辛子）／加工デンプン、調味料（アミノ酸等）、カラメル色素、炭酸カルシウム、かんすい、増粘多糖類、ソルビット、酒精、香料、グリセリン、カロチノイド色素、酸化防止剤（ビタミンＥ）、酸味料、甘味料（スクラロース）、ビタミンＢ２、ビタミンＢ１、（一部に卵･乳成分･小麦･えび･ごま･大豆･鶏肉･豚肉を含む）</t>
+  </si>
+  <si>
+    <t>油揚げめん（小麦粉（国内製造）、植物油脂、食塩、オニオン粉末）、ソース（ペッパーガーリックマヨネーズ、しょうゆ、糖類、豚脂、植物油脂、食塩、ポークエキス、香味油、たん白加水分解物、香味調味料、香辛料、醸造酢）、かやく（キャベツ）、ふりかけ（香辛料、アオサ、赤唐辛子）／調味料（アミノ酸等）、かんすい、炭酸カルシウム、酒精、香料、増粘剤（キサンタンガム）、乳化剤、酸味料、カロチノイド色素、酸化防止剤（ビタミンＥ）、カラメル色素、香辛料抽出物、炭酸マグネシウム、ビタミンＢ２、ビタミンＢ１、（一部に卵･乳成分･小麦･ごま･大豆･鶏肉･豚肉を含む）</t>
+  </si>
+  <si>
+    <t>油揚げめん（小麦粉（国内製造）、植物油脂、食塩、オニオン粉末）、ソース（半固体状ドレッシング、しょうゆ、糖類、豚脂、食塩、ポークエキス、魚醤、魚介エキス、たん白加水分解物、香味調味料、香辛料）、かやく（キャベツ）、ふりかけ（たらこ加工品、のり、香辛料）／調味料（アミノ酸等）、かんすい、炭酸カルシウム、カラメル色素、酒精、香料、増粘剤（加工デンプン、キサンタンガム）、乳化剤、酸味料、カロチノイド色素、ベニコウジ色素、酸化防止剤（ビタミンＥ）、香辛料抽出物、炭酸マグネシウム、ビタミンＢ２、ビタミンＢ１、（一部に卵･乳成分･小麦･いか･さけ･さば･大豆･豚肉を含む）</t>
+  </si>
+  <si>
+    <t>麺［米粉（国産）、馬鈴薯でん粉／加工デンプン、アルギン酸エステル、ビタミンＢ２］、スープ［みそ、しょうゆ、植物油脂、発酵調味料、にんにく、砂糖、食塩、すりごま、たん白加水分解物、酵母エキス、香辛料／酒精、カラメル色素、調味料（有機酸等）、酸味料、（一部に大豆・ごまを含む］</t>
+  </si>
+  <si>
+    <t>麺［米粉（国産）、馬鈴薯でん粉／加工デンプン、アルギン酸エステル、ビタミンＢ２］、スープ［クリーミングパウダー、発酵調味料、食塩、たん白加水分解物、しょうゆ、植物油脂、砂糖、酵母エキス、ハクサイエキスパウダー、ガーリックパウダー、醸造酢、香辛料／カラメル色素、増粘剤（グァーガム）、調味料（有機酸等）、（一部に乳・大豆を含む］</t>
+  </si>
+  <si>
+    <t>油揚げめん（小麦粉（国内製造）、植物油脂、食塩、しょうゆ）、ソース（砂糖、食塩、ソース、香辛料、デキストリン、たん白加水分解物）、かやく（キャベツ）/加工でんぷん、調味料（アミノ酸等）、カラメル色素、炭酸Ca、かんすい、酸味料、増粘多糖類、炭酸Mg、酸化防止剤（ビタミンE）、香料、ビタミンB2、ビタミンB1、（一部に小麦・大豆・ごまを含む）</t>
+  </si>
+  <si>
+    <t>チョコレート（砂糖、全粉乳、植物油脂、ココアバター、カカオマス、乳糖）、ウエハース（小麦粉、砂糖、でんぷん、植物油脂、食塩）／加工でんぷん、乳化剤（大豆由来）貝カルシウム、香料、着色料（カラメル）、膨張剤</t>
+  </si>
+  <si>
+    <t>小麦粉・ショートニング・砂糖・全粒粉・乳糖・乳頭を主原料とする食品・乾燥全卵・でんぷん・食塩・膨張剤・香料・乳化剤</t>
+  </si>
+  <si>
+    <t>小麦粉・ショートニング・砂糖・ココアパウダー・乳糖・乳糖を主原料とする食品・乾燥全卵・でんぷん・食塩・炭酸カルシウム 膨張剤・香料・乳化剤</t>
+  </si>
+  <si>
+    <t>野菜（じゃがいも（国産）、にんじん、コーン）、大豆油、豚肉、小麦粉ルウ、ソテーオニオン、砂糖、カレー粉、エキス（ポーク、酵母）、醤油、トマトペースト、食塩、チキンエキス調味料、ミルポワペースト、チーズパウダー、酵母エキスパウダー／増粘剤（加工でん粉）、調味料（アミノ酸等）、セルロース、（一部に乳成分・小麦・大豆・鶏肉・豚肉を含む）</t>
+  </si>
+  <si>
+    <t>欄外裏面に記載［たまご］小麦粉（国内製造）、いりごま、乳糖、砂糖、卵黄粉末、食塩、加工油脂、すりごま、大豆加工品、鰹削り節、こしあん、還元水あめ、エキス（チキン、酵母、鰹節、魚介）、鶏肉粉末、みそ、海藻カルシウム、のり、醤油、鶏脂、乳製品、ぶどう糖果糖液糖、イースト、みりん、あおさ、抹茶、デキストリン／調味料（アミノ酸）、卵殻カルシウム、酸化防止剤（ビタミンＥ）、カロチノイド色素、香料、（一部に卵・乳成分・小麦・ごま・大豆・鶏肉を含む）［さけ］いりごま（国内製造）、乳糖、大豆加工品、砂糖、食塩、小麦粉、加工油脂、鮭、すりごま、卵黄粉末、還元水あめ、こしあん、海藻カルシウム、エキス（チキン、酵母）、鶏肉粉末、みそ、香味油、のり、鶏脂、醤油、乳製品、ぶどう糖果糖液糖、イースト／調味料（アミノ酸等）、卵殻カルシウム、着色料（紅麹、カロチノイド）、酸化防止剤（ビタミンＥ）、香料、（一部に卵・乳成分・小麦・ごま・さけ・大豆・鶏肉を含む）［おかか］いりごま（国内製造）、乳糖、鰹削り節、砂糖、食塩、小麦粉、すりごま、加工油脂、醤油、還元水あめ、大豆加工品、卵黄粉末、鰹節粉、エキス（チキン、鰹節、酵母</t>
+  </si>
+  <si>
+    <t>スイートコーンパウダー（アメリカ製造）、でん粉、砂糖、デキストリン、食塩、全粉乳、乳糖、脱脂粉乳、エキス（チキン、酵母、オニオン）、うきみ（クラッカー）／調味料（アミノ酸）、膨張剤、カカオ色素、（一部に乳成分・小麦・鶏肉を含む）</t>
+  </si>
+  <si>
+    <t>野菜（じゃがいも（国産）、にんじん）、ソテーオニオン、豚肉、砂糖、エキス（ポーク、酵母）、カレー粉、トマトペースト、ポテト粉末、食塩、なたね油、かぼちゃペースト、ほうれん草ペースト、コーンペースト／増粘剤（加工でん粉）、（一部に豚肉を含む）</t>
+  </si>
+  <si>
+    <t>野菜（じゃがいも、にんじん、コーン、玉ねぎ、かぼちゃ、グリーンアスパラガス）、豚肉、小麦粉、マーガリン、はちみつ、砂糖、カレー粉、食塩、エキス（ポーク、酵母）、豚脂、トマトペースト、チーズ、コーン油、増粘剤（加工澱粉）、調味料（アミノ酸）、セルロース、（原材料の一部に大豆を含む）</t>
+  </si>
+  <si>
+    <t>鶏肉（国産）、鶏卵、玉ねぎ、砂糖、発酵調味料、食塩、醤油、エキス（チキン、酵母）、鰹節粉、鶏脂／増粘剤（加工でん粉、キサンタン）、調味料（アミノ酸等）、トレハロース、カロチノイド色素、（一部に卵・小麦・大豆・鶏肉を含む）</t>
+  </si>
+  <si>
+    <t>トマトペースト（ポルトガル製造）、砂糖、ミルポワペースト、ウスターソース、りんごペースト、小麦粉ルウ、ソテーオニオン、チキンエキス、大豆油、食塩、粒状植物性たん白、牛肉、酵母エキスパウダー、かぼちゃペースト、グリーンアスパラガスペースト、コーンペースト／増粘剤（加工でん粉）、調味料（アミノ酸）、カラメル色素、（一部に小麦・牛肉・大豆・鶏肉・りんごを含む）</t>
+  </si>
+  <si>
+    <t>小麦粉（国内製造）、マーガリン、砂糖、小麦全粒粉、発酵風味液、食塩、殺菌乳酸菌末／香料、カロテン色素、（一部に小麦・乳成分・大豆を含む）</t>
+  </si>
+  <si>
+    <t>砂糖（国内製造）、ぶどう糖、水あめ、ゼラチン、ウーロン茶抽出物／ガムベース、酸味料、軟化剤、香料、ビタミンＣ、クチナシ色素</t>
+  </si>
+  <si>
+    <t>砂糖（国内製造）、小麦粉、植物油脂、全粉乳、乳糖、カカオマス、ホエイパウダー、クッキークランチ、ココアパウダー、でん粉、ショートニング、食塩／乳化剤（大豆由来）、カラメル色素、膨脹剤、香料</t>
+  </si>
+  <si>
+    <t>砂糖（国内製造、外国製造）、小麦粉、植物油脂、乳糖、でん粉、ショートニング、ココアバター、全粉乳、ホエイパウダー、液卵、小麦全粒粉、乳等を主要原料とする食品（はっ酵バター、植物油脂、バターオイル、脱脂粉乳、食塩）、脱脂粉乳、クリームパウダー、食塩／膨脹剤、カラメル色素、香料、乳化剤（大豆由来）</t>
+  </si>
+  <si>
+    <t>水飴（国内製造）、砂糖、ゼラチン、でんぷん／ソルビトール、酸味料、マンニトール、増粘剤（ペクチン）、香料、光沢剤、着色料(アントシアニン、クチナシ、紅麹、カラメル、紅花黄、カロチン)、乳化剤、（一部にゼラチンを含む） 本品製造ラインでは、乳成分を含む製品を生産しています。</t>
+  </si>
+  <si>
+    <t>【青リンゴ】砂糖（国内製造）、水飴、ゼラチン、果糖ぶどう糖液糖、濃縮青リンゴ果汁／酸味料、ゲル化剤（ペクチン）、香料、光沢剤、着色料（黄色４号、青色１号）、（一部にりんご・ゼラチンを含む）　【レモン】砂糖（国内製造）、水飴、ゼラチン、果糖ぶどう糖液糖、濃縮レモン果汁／酸味料、香料、ゲル化剤（ペクチン）、光沢剤、着色料（黄色４号）、（一部にゼラチンを含む）　【グレープ】砂糖（国内製造）、水飴、ゼラチン、果糖ぶどう糖液糖、濃縮グレープ果汁／酸味料、香料、ゲル化剤（ペクチン）、光沢剤、甘味料（アセスルファムＫ、ステビア）、着色料（赤色４０号、青色１号）、（一部にゼラチンを含む）　【イチゴ】砂糖（国内製造）、水飴、ゼラチン、果糖ぶどう糖液糖、濃縮イチゴ果汁／酸味料、ゲル化剤（ペクチン）、香料、光沢剤、着色料（赤色４０号）、（一部にゼラチンを含む）</t>
+  </si>
+  <si>
+    <t>ポテトフレーク（アメリカ製造又はドイツ製造又はその他）、植物油脂、甘えびパウダー、食塩／加工デンプン、乳化剤、調味料（アミノ酸）、（一部にえびを含む）</t>
+  </si>
+  <si>
+    <t>小麦粉、砂糖、植物油脂、ココアパウダー、コーンスターチ、食塩／膨張剤、乳化剤、香料、酸化防止剤（V．Ｅ、V．Ｃ）、（原材料の一部に小麦・乳成分・大豆を含む）</t>
+  </si>
+  <si>
+    <t>小麦粉、砂糖、植物油脂、ココアパウダー、コーンスターチ、食塩／膨張剤、乳化剤、香料、酸味料、酸化防止剤（Ｖ．Ｃ、Ｖ．Ｅ）、（一部に小麦・大豆を含む）</t>
+  </si>
+  <si>
+    <t>準チョコレート（砂糖、植物油脂（大豆を含む）、全粉乳、乳糖、カカオマス、ココアパウダー）（国内製造）、小麦粉、鶏卵、砂糖、デキストリン、ショートニング、食塩/乳化剤（大豆由来）、膨張剤、香料</t>
+  </si>
+  <si>
+    <t>小麦粉（国内製造）、砂糖、チョコレート（乳成分を含む）、ショートニング（大豆を含む）、還元水あめ、白練餡（生餡、砂糖、水あめ、還元麦芽糖水あめ）、ココアパウダー、大豆粉、鶏卵加工品（鶏卵、砂糖）、水あめ、脱脂粉乳、卵黄粉末（卵を含む）、卵黄粉末（卵を含む）、全粉乳、でん粉分解物、カカオマス、食塩、酵母エキス／加工でん粉、乳化剤（大豆由来）、香料、膨脹剤</t>
+  </si>
+  <si>
+    <t>植物油脂（国内製造）（大豆を含む）、砂糖、砂糖粉乳調製品（砂糖、全粉乳、脱脂粉乳、ココアバター）、乳糖、カカオマス、全粉乳、ココアバター、脱脂粉乳／乳化剤（大豆由来）、香料（乳由来）</t>
+  </si>
+  <si>
+    <t>砂糖（外国製造、国内製造）、全粉乳、乳糖、小麦粉、植物油脂、カカオマス、ココアバター、ココアパウダー、イースト／乳化剤、アラビアガム、光沢剤、重曹、イーストフード、香料、（一部に小麦・乳成分・大豆を含む）</t>
+  </si>
+  <si>
+    <t>砂糖（外国製造、国内製造）、全粉乳、乳糖、植物油脂、小麦粉、カカオマス、ココアバター、いちご果汁パウダー、イースト、ココアパウダー／乳化剤、酸味料、アラビアガム、香料、光沢剤、重曹、イーストフード、（一部に小麦・乳成分・大豆を含む）</t>
+  </si>
+  <si>
+    <t>カカオマス（コートジボワール製造又は国内製造又はその他）、砂糖、小麦粉、乳糖、植物油脂、ココアバター、カカオニブ、ココアパウダー、全粉乳、イースト／乳化剤、アラビアガム、光沢剤、重曹、イーストフード、香料、（一部に小麦・乳成分・大豆を含む</t>
+  </si>
+  <si>
+    <t>チョコレートコーチング（植物油脂、砂糖、乳糖、全粉乳、ココアバター）（国内製造）、ビスケット（小麦粉、砂糖、ショートニング、食塩）、小麦粉、乳糖、植物油脂、砂糖、いちご果汁パウダー、乾燥いちご加工品、イースト、ココアパウダー、全粉乳、カカオマス、ココアバター／乳化剤、酸味料、膨脹剤、香料、着色料（赤ビート、紅麹）、重曹、イーストフード、（一部に小麦・乳成分・大豆を含む）</t>
+  </si>
+  <si>
+    <t>チョコレートコーチング（植物油脂、砂糖、乳糖、全粉乳、ココアバター）（国内製造）、ビスケット（小麦粉、砂糖、ショートニング、食塩）、小麦粉、植物油脂、乳糖、抹茶、砂糖、ココアパウダー、緑茶、全粉乳、カカオマス、イースト、ココアバター／乳化剤、膨脹剤、香料、重曹、イーストフード、（一部に小麦・乳成分・大豆を含む）</t>
+  </si>
+  <si>
+    <t>植物油脂（国内製造）、ビスケット（小麦粉、砂糖、ショートニング、ココアパウダー、食塩）、砂糖、小麦粉、カカオマス、乳糖、全粉乳、ココアバター、ココアパウダー、イースト／乳化剤、膨脹剤、香料、重曹、イーストフード、（一部に小麦・乳成分・大豆を含む）</t>
+  </si>
+  <si>
+    <t>チョコレートコーチング（植物油脂、砂糖、乳糖、全粉乳、ココアバター）（国内製造）、全粒粉ビスケット（小麦粉、小麦全粒粉、砂糖、ショートニング、食塩）、小麦粉、乳糖、砂糖、植物油脂、全粉乳、カカオマス、ココアバター、ココアパウダー、イースト／乳化剤（大豆由来）、膨脹剤、カラメル色素、香料、重曹、イーストフード</t>
+  </si>
+  <si>
+    <t>砂糖（外国製造、国内製造）、全粉乳、乳糖、カカオマス、小麦粉、植物油脂、ココアバター、オレンジ果汁パウダー、イースト、ココアパウダー／乳化剤、香料、酸味料、重曹、イーストフード、（一部に小麦・乳成分・オレンジ・大豆を含む）</t>
+  </si>
+  <si>
+    <t>牛乳、砂糖、コーヒー、脱脂粉乳／乳化剤</t>
+  </si>
+  <si>
+    <t>コーングリッツ（国内製造）、植物油、デキストリン、砂糖、食塩、ぶどう糖、チーズパウダー、酵母エキスパウダー、たんぱく質濃縮ホエイパウダー、赤唐辛子パウダー、、オニオンパウダー/香料、調味料（アミノ酸等）、着色料（カロチノイド、カラメル）、酸味料、（一部に乳成分・大豆を含む）</t>
+  </si>
+  <si>
+    <t>油揚げめん（小麦粉(国内製造)、植物油脂、でん粉、食塩、しょうゆ、たん白加水分解物）、スープ（糖類、食塩、しょうゆ、貝エキス、野菜粉末、チキンエキス、ポークエキス、えびエキス、香辛料、たん白加水分解物）、かやく（かまぼこ、コーン）／調味料（アミノ酸等）、加工でん粉、炭酸カルシウム、カラメル色素、かんすい、増粘多糖類、酸味料、酸化防止剤（ビタミンＥ）、クチナシ色素、イカスミ色素、ビタミンＢ２、ビタミンＢ１、ベニコウジ色素、（一部にえび・小麦・乳成分・いか・大豆・鶏肉・豚肉を含む）</t>
+  </si>
+  <si>
+    <t>油揚げめん（小麦粉、植物油脂、でん粉、食塩、しょうゆ、たん白加水分解物）、スープ（糖類、食塩、しょうゆ、貝エキス、香辛料、チキンエキス、ポークエキス、えびエキス、たん白加水分解物）、かやく（かまぼこ、コーン、ねぎ）、調味料（アミノ酸等）、加工でん粉、炭酸カルシウム、カラメル色素、かんすい、増粘多糖類、酸味料、酸化防止剤（ビタミンＥ）、クチナシ色素、イカスミ色素、ビタミンＢ２、ベニコウジ色素、ビタミンＢ１</t>
+  </si>
+  <si>
+    <t>油揚げめん（小麦粉、植物油脂、でん粉、食塩、大豆食物繊維）、スープ（しょうゆ、食塩、たん白加水分解物、ポークエキス、糖類、豚脂、植物油脂、かつお節エキス、酵母エキス、香辛料、煮干いわし粉末）、かやく（チャーシュー、メンマ、ナルト、ねぎ）、調味料（アミノ酸等）、酒精、カラメル色素、炭酸カルシウム、香料、かんすい、増粘剤（キサンタン）、レシチン、クチナシ色素、酸化防止剤（ビタミンＥ）、ビタミンＢ２、ビタミンＢ１、ベニコウジ色素、（原材料の一部に卵、乳成分を含む）</t>
+  </si>
+  <si>
+    <t>油揚げめん（小麦粉、植物油脂、でん粉、食塩、粉末卵、糖類）、スープ（みそ、食塩、糖類、ポークエキス、コチュジャン、植物油脂、豚脂、豆板醤、香辛料、香味食用油、調味油脂、たん白加水分解物）、かやく（ねぎ、鶏・豚味付肉そぼろ、コーン）、加工でん粉、調味料（アミノ酸等）、酒精、炭酸カルシウム、カラメル色素、香料、クチナシ色素、かんすい、増粘剤（キサンタン）、酸味料、酸化防止剤（ビタミンＥ、ローズマリー抽出物）、ビタミンＢ2、ビタミンＢ１、香辛料抽出物、（原材料の一部にごまを含む）</t>
+  </si>
+  <si>
+    <t>油揚げめん（小麦粉、植物油脂、でん粉、食塩、みそ、糖類）、スープ（豚脂、しょうゆ、食塩、糖類、ポークエキス、チキンエキス、たん白加水分解物、植物油脂、香辛料、酵母エキス）、かやく（チャーシュー、ねぎ）、加工でん粉、調味料（アミノ酸等）、酒精、カラメル色素、炭酸カルシウム、かんすい、レシチン、クチナシ色素、増粘剤（キサンタン）、香料、酸化防止剤（ビタミンＥ）、ビタミンＢ２、ビタミンＢ１、（原材料の一部に卵、乳成分を含む）</t>
+  </si>
+  <si>
+    <t>油揚げめん（小麦粉、植物油脂、食塩）、ソース（ソース、糖類、食塩、豚脂、植物油脂、香辛料、たん白加水分解物、香味調味料）、かやく（キャベツ）、カラメル色素、調味料（アミノ酸等）、炭酸カルシウム、かんすい、酸味料、酸化防止剤（ビタミンＥ）、香料、増粘剤（キサンタン）、ビタミンＢ２、ビタミンＢ１、（原材料の一部に乳成分、大豆、りんご、ゼラチンを含む）</t>
+  </si>
+  <si>
+    <t>砂糖（国内製造）、水飴、果汁（いちご、パインアップル、レモン、オレンジ、りんご、メロン、ぶどう、もも）/酸味料、香料、着色料（アントシアニン、パプリカ色素、カロチン、クチナシ、紅麹、紅花黄）、（一部にオレンジ・もも・りんごを含む）</t>
+  </si>
+  <si>
+    <t>ぶどう糖、砂糖、水あめ、還元水あめ、ガムベース、酸味料、香料、乳酸カルシウム、軟化剤、アントシアニン色素、緑茶抽出物</t>
+  </si>
+  <si>
+    <t>砂糖(国内製造)､ぶどう糖､水あめ､還元水あめ､ 酵母エキス､デキストリン／ガムベース､酸味料､ 香料､軟化剤､カロチノイド色素</t>
+  </si>
+  <si>
+    <t>ぶどう糖、砂糖、水あめ、還元水あめ/ガムベース、酸味料、香料、軟化剤、着色料（クチナシ、フラボノイド）</t>
+  </si>
+  <si>
+    <t>砂糖（国内製造）､ぶどう糖、水あめ､還元水あめ ／ガムベース、酸味料、香料</t>
+  </si>
+  <si>
+    <t>砂糖､ぶどう糖、水あめ､還元水あめ／ガムベース、酸味料、香料</t>
+  </si>
+  <si>
+    <t>ぶどう糖(国内製造)､砂糖､水あめ､還元水あめ ／ガムベース､酸味料､香料､カラメル色素、軟化剤</t>
+  </si>
+  <si>
+    <t>ぶどう糖(国内製造)､砂糖､水あめ､還元水あめ、濃縮ぶどう果汁 ／ガムベース､酸味料､香料､アントシアニン色素</t>
+  </si>
+  <si>
+    <t>砂糖(国内製造)､ぶどう糖、水あめ／ガムベース､酸味料､ 糊料(アラビアガム)､香料､着色料(フラボノイド、アントシアニン)､光沢剤</t>
+  </si>
+  <si>
+    <t>果糖ぶどう糖液糖（国内製造）、もも果汁、脱脂粉乳、乳酸菌飲料、ピーチソース／酸味料、安定剤（大豆多糖類）、香料、甘味料（アスパルテーム・Ｌ－フェニルアラニン化合物、アセスルファムＫ）、ベニバナ黄色素、野菜色素</t>
+  </si>
+  <si>
+    <t>米めん（ベトナム製造（米、でん粉、食塩））、スープ（食塩、砂糖、鶏油、香味油、たん白加水分解物、植物油脂、チキンエキス、香辛料、酵母エキス、チキン調味料、ネギエキス）、かやく（大豆加工品、ねぎ、もやし、コリアンダー）／加工でん粉、調味料（アミノ酸等）、酒精、増粘剤（加工でん粉、増粘多糖類）、香料、カラメル色素、乳化剤、酸味料、酸化防止剤（ビタミンＥ）、（一部に乳成分・大豆・鶏肉・豚肉を含む）</t>
+  </si>
+  <si>
+    <t>米めん（ベトナム製造（米、でん粉、食塩））、かやく入りスープ（食塩、チンゲン菜、砂糖、トムヤムシーズニングパウダー、大豆加工品、香辛料、ねぎ、酵母エキス、たん白加水分解物、蝦醤、チキン調味料、エビエキス、コリアンダー、唐辛子）／加工でん粉、調味料（アミノ酸等）、酸味料、香料、微粒二酸化ケイ素、カロチノイド色素、甘味料（スクラロース、アセスルファムＫ）、乳化剤、増粘剤（グァーガム）、（一部にえび・大豆・鶏肉・ゼラチンを含む）</t>
+  </si>
+  <si>
+    <t>米めん（ベトナム製造（米、でん粉、食塩））、スープ（たん白加水分解物、糖類、食塩、香辛料、牛脂、発酵調味料、植物油脂、醸造酢、トマトケチャップ、ビーフエキス、香味油、酵母エキス）、かやく（大豆加工品、ねぎ、唐辛子）／加工でん粉、調味料（アミノ酸等）、酒精、香料、香辛料抽出物、増粘多糖類、カラメル色素、乳化剤、酸味料、甘味料（スクラロース、アセスルファムＫ）、酸化防止剤（ビタミンＥ）、（一部にえび・牛肉・大豆を含む）</t>
+  </si>
+  <si>
+    <t>小麦粉（国内製造）、ショートニング、砂糖、チョコレートチップ、でん粉、鶏卵、ココアパウダー、食塩、スパイス／膨張剤、乳化剤、香料、カロテン色素、（一部に小麦・卵・乳成分・大豆を含む）</t>
+  </si>
+  <si>
+    <t>果実（りんご、オレンジ、グァバ、パインアップル、パッションフルーツ）、砂糖類（砂糖、ぶどう糖）、高麗人参根エキス、Ｌ－カルニチンＬ－酒石酸塩、植物油、塩化Ｎａ、ガラナ種子エキス／炭酸、クエン酸、香料、保存料（安息香酸Ｎａ）、Ｌ－アルギニン、クエン酸Ｎａ、カフェイン、甘味料（スクラロース）、ナイアシン、イノシトール、ビタミンＢ６、ビタミンＢ２、着色料（β－カロテン）、ビタミンＢ１２</t>
+  </si>
+  <si>
+    <t>砂糖類（砂糖、ぶどう糖）、高麗人参根エキス、Ｌ‐カルニチンＬ‐酒石酸塩、塩化Ｎａ、　　　　　　　ガラナ種子エキス、クエン酸、香料、甘味料（Ｄ‐リボース、スクラロース）、Ｌ‐アルギニン、　　　　クエン酸Ｎａ、カフェイン、保存料（安息香酸）、ナイアシン、着色料（アントシアニン）、　　　　　イノシトール、Ｖ．Ｂ６、Ｖ．Ｂ２、Ｖ．Ｂ１２</t>
+  </si>
+  <si>
+    <t>牛乳（国内製造）、砂糖、コーヒー、脱脂粉乳、全粉乳、デキストリン／乳化剤、香料、セルロース</t>
+  </si>
+  <si>
+    <t>馬鈴薯(日本:遺伝子組換えでない)、植物油、香味油、砂糖、ぶどう糖、ブラックペパー、でん粉、粉末しょうゆ(小麦・大豆を含む)、食塩、オニオン、魚介エキスパウダー、酵母エキスパウダー/調味料(アミノ酸等)、香辛料抽出物、香料</t>
+  </si>
+  <si>
+    <t>生地(国内製造)(小麦粉、でん粉、ほたてエキスパウダー、えびパウダー、あさりエキスパウダー、砂糖、粉末しょうゆ、植物油、しじみペーストパウダー、かきエキスパウダー)、植物油、デキストリン、ぶどう糖、あさりエキスパウダー、粉末しょうゆ、いわしエキスパウダー、酒粕パウダー、食塩、唐辛子、乳糖/加工デンプン、トレハロース、調味料(アミノ酸等)、酸味料、香料、(一部に乳成分・小麦・えび・かに・さば・大豆・ゼラチンを含む)</t>
+  </si>
+  <si>
+    <t>乾燥ポテト（外国製造）、植物油脂、サワークリームオニオン風味パウダー（食塩、ホエイパウダー（乳製品）、砂糖、オニオンパウダー、粉末酢、たんぱく加水分解物、ねぎエキスパウダー、デキストリン、酵母エキスパウダー）、食塩、オニオンパウダー、粉末油脂、砂糖、澱粉／加工澱粉、トレハロース、調味料（アミノ酸等）、増粘剤（カードラン）、酸味料、香料、炭酸Ca、香辛料抽出物、甘味料（スクラロース、ステビア）、酸化防止剤（ビタミンE）、（一部に乳成分を含む）</t>
+  </si>
+  <si>
+    <t>乾燥ポテト（外国製造）、植物油脂、食塩、砂糖、ポテト風味パウダー（デキストリン、食塩、ポテトパウダー、醤油風味調味料、酵母エキスパウダー、粉末香味油、ビーフ風味パウダー、香味油）、ブドウ糖、粉末油脂、ビーフ風味パウダー（ビーフエキスパウダー、食塩、たんぱく加水分解物、ビーフ風味調味料、乳糖、野菜エキスパウダー、香辛料）、澱粉、酵母エキスパウダー／加工澱粉、トレハロース、調味料（アミノ酸等）、増粘剤（カードラン）、炭酸Ca、香料、甘味料（スクラロース）、酸化防止剤（ビタミンE）、酸味料、（一部に乳成分・小麦・牛肉・大豆・鶏肉・豚肉を含む）</t>
+  </si>
+  <si>
+    <t>乾燥ポテト（外国製造）、植物油脂、コーングリッツ、小麦粉、粉末油脂、食塩、砂糖、ポテト風味パウダー（デキストリン、食塩、ポテトパウダー、醤油風味調味料、酵母エキスパウダー、粉末香味油、ビーフ風味パウダー、香味油）、ブドウ糖、ビーフオイル、澱粉、酵母エキスパウダー／トレハロース、セルロース、調味料（アミノ酸等）、香料、卵殻Ca、増粘剤（カードラン）、乳化剤、炭酸Ca、酸味料、（一部に卵・乳成分・小麦・牛肉・大豆・鶏肉・豚肉を含む）</t>
+  </si>
+  <si>
+    <t>コーングリッツ（国内製造）、植物油脂、砂糖、マーガリン、加糖れん乳、食塩、卵黄粉末／ソルビトール、香料、卵殻Ca、乳化剤、甘味料（スクラロース）、カロチノイド色素、（一部に卵・乳成分・大豆を含む）</t>
+  </si>
+  <si>
+    <t>小麦粉、砂糖、植物油脂、全粉乳、ココアバター、ライ麦粉、ショートニング、脱脂粉乳、麦芽エキス、いちごパウダー、バター風味調味料、練乳加工品、カラメルソース、食塩、乳化剤、膨脹剤、香料、着色料（ビートレッド、カラメル）、酸味料、（一部に小麦・乳成分・大豆を含む）</t>
+  </si>
+  <si>
+    <t>砂糖（国内製造）、ぶどう糖、水飴、でん粉／ガムベース、酸味料、軟化剤、香料、着色料（クチナシ）</t>
+  </si>
+  <si>
+    <t>〈グレープ〉砂糖（国内製造）、水あめ、グレープペースト/酸味料、香料、着色料（アントシアニン、クチナシ）、チャ抽出物 〈オレンジ〉砂糖（国内製造）、水あめ、オレンジペースト/酸味料、香料、着色料（カロテノイド）、チャ抽出物 〈ストロベリー〉砂糖（国内製造）、水あめ、ストロベリーペースト/酸味料、香料、着色料（アントシアニン、カロテノイド）、チャ抽出物 〈メロン〉砂糖（国内製造）、水あめ、濃縮メロン果汁/酸味料、着色料（紅麹、クチナシ）、香料、チャ抽出物</t>
+  </si>
+  <si>
+    <t>アンパンマン：砂糖、全粉乳、植物油脂、カカオマス、ココアバター、乳糖、脱脂粉乳、乳化剤（大豆由来）、香料。ばいきんまん：砂糖、植物油脂、全粉乳、ココアバター、カカオマス、乳糖、脱脂粉乳、乳化剤（大豆由来）、野菜色素、香料。ドキンちゃん：砂糖、植物油脂、全粉乳、ココアバター、カカオマス、乳糖、脱脂粉乳、乳化剤（大豆由来）、野菜色素、香料</t>
+  </si>
+  <si>
+    <t>ビスケット（小麦粉、砂糖、植物油脂、その他：乳を含む）、砂糖、カカオマス、全粉乳、植物油脂、ココアバター、水あめ、膨脹剤、乳化剤（大豆由来）、光沢剤、卵殻カルシウム、香料</t>
+  </si>
+  <si>
+    <t>砂糖(外国製造又は国内製造)、全粉乳、植物油脂、カカオマス、ココアバター、乳糖、脱脂粉乳、油脂加工品／乳化剤(大豆由来)、野菜色素、香料(乳・大豆由来)</t>
+  </si>
+  <si>
+    <t>小麦粉（国内製造）、砂糖、植物油脂、チョコレートチップ（乳成分を含む）、還元水あめ、白ねりあん（乳成分を含む）、卵、全脂大豆粉、カカオマス、水あめ、脱脂粉乳、食塩、卵黄（卵を含む）、全粉乳／加工デンプン、乳化剤（乳・大豆由来）、香料（乳・大豆由来）、安定剤（加工デンプン）、膨脹剤、カラメル色素</t>
+  </si>
+  <si>
+    <t>小麦粉（国内製造）、砂糖、植物油脂、バター、全粉乳、発酵種（小麦を含む）、食塩、乳等を主原料とする食品/乳化剤（小麦・大豆由来）、香料（乳・大豆由来）、カロテノイド色素</t>
+  </si>
+  <si>
+    <t>水飴（国内製造）、砂糖、ゼラチン、粉末オブラート／ソルビット、酸味料、糊料（ペクチン）、光沢剤、香料、乳化剤、着色料（クチナシ、野菜色素、紅花黄、パプリカ色素）</t>
   </si>
 </sst>
 </file>
@@ -868,11 +774,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E615D68-CAB4-47E0-941D-23CC2B10D297}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:A164"/>
+  <dimension ref="A1:A145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -886,122 +790,117 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
@@ -1011,696 +910,565 @@
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>69</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>70</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>78</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>80</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>81</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>82</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>84</v>
+        <v>29</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>88</v>
+        <v>15</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>4</v>
+        <v>82</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>102</v>
+        <v>18</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>103</v>
+        <v>17</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>104</v>
+        <v>17</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>156</v>
+        <v>98</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>157</v>
+        <v>24</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>122</v>
+        <v>19</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>123</v>
+        <v>25</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>130</v>
+        <v>35</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>132</v>
+        <v>34</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>138</v>
+        <v>22</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>139</v>
+        <v>20</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>140</v>
+        <v>30</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>141</v>
+        <v>21</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>49</v>
+        <v>116</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>55</v>
+        <v>118</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>8</v>
+        <v>120</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>144</v>
+        <v>13</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>145</v>
+        <v>28</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>6</v>
+        <v>122</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>7</v>
+        <v>123</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>53</v>
+        <v>124</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>57</v>
+        <v>125</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>58</v>
+        <v>126</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>17</v>
+        <v>127</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>47</v>
+        <v>128</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>48</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A82" xr:uid="{8E615D68-CAB4-47E0-941D-23CC2B10D297}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>